<commit_message>
Model Updated to Function with FSN Design
- Updated all muscle stimulus tension curves ensure that desired activations can be achieved in the range of [-60,-40] mV
- Implemented thresholding to the synergy activation profiles, allowing users to filter out low-contributing muscles from synergies
- Sum of sines fit now iterates up to the minimum number of sine waves to satisfy a given condition rather than defaulting to eight sine waves
</commit_message>
<xml_diff>
--- a/ParameterCalculation/MuscleParameters_20190513.xlsx
+++ b/ParameterCalculation/MuscleParameters_20190513.xlsx
@@ -645,28 +645,28 @@
         <v>167.14908328759071</v>
       </c>
       <c r="I2">
-        <v>26.376000000000001</v>
+        <v>21.984396</v>
       </c>
       <c r="J2">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L2">
+        <v>-60</v>
+      </c>
+      <c r="M2">
+        <v>-40</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>21.984396</v>
+      </c>
+      <c r="P2">
         <v>1.0740679384557621</v>
-      </c>
-      <c r="M2">
-        <v>2.1481358769115242</v>
-      </c>
-      <c r="N2">
-        <v>3.2222038153672861</v>
-      </c>
-      <c r="O2">
-        <v>1.0740679384557621</v>
-      </c>
-      <c r="P2">
-        <v>21.97944</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -695,28 +695,28 @@
         <v>19.550246544346372</v>
       </c>
       <c r="I3">
-        <v>2.2440000000000002</v>
+        <v>1.870374</v>
       </c>
       <c r="J3">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L3">
+        <v>-60</v>
+      </c>
+      <c r="M3">
+        <v>-40</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1.870374</v>
+      </c>
+      <c r="P3">
         <v>0.6819514577231951</v>
-      </c>
-      <c r="M3">
-        <v>1.3639029154463902</v>
-      </c>
-      <c r="N3">
-        <v>2.0458543731695853</v>
-      </c>
-      <c r="O3">
-        <v>0.6819514577231951</v>
-      </c>
-      <c r="P3">
-        <v>1.8698399999999999</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -745,28 +745,28 @@
         <v>26.352679558744015</v>
       </c>
       <c r="I4">
-        <v>6.5159999999999991</v>
+        <v>5.4310859999999996</v>
       </c>
       <c r="J4">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L4">
+        <v>-60</v>
+      </c>
+      <c r="M4">
+        <v>-40</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>5.4310859999999996</v>
+      </c>
+      <c r="P4">
         <v>1.4754747575459182</v>
-      </c>
-      <c r="M4">
-        <v>2.9509495150918363</v>
-      </c>
-      <c r="N4">
-        <v>4.426424272637755</v>
-      </c>
-      <c r="O4">
-        <v>1.4754747575459182</v>
-      </c>
-      <c r="P4">
-        <v>5.4331200000000006</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -795,28 +795,28 @@
         <v>16.59695451932242</v>
       </c>
       <c r="I5">
-        <v>7.3199999999999994</v>
+        <v>6.1012199999999996</v>
       </c>
       <c r="J5">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L5">
+        <v>-60</v>
+      </c>
+      <c r="M5">
+        <v>-40</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>6.1012199999999996</v>
+      </c>
+      <c r="P5">
         <v>2.6026604179888015</v>
-      </c>
-      <c r="M5">
-        <v>5.2053208359776031</v>
-      </c>
-      <c r="N5">
-        <v>7.8079812539664051</v>
-      </c>
-      <c r="O5">
-        <v>2.6026604179888015</v>
-      </c>
-      <c r="P5">
-        <v>6.10344</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -845,28 +845,28 @@
         <v>74.645209347716573</v>
       </c>
       <c r="I6">
-        <v>26.963999999999999</v>
+        <v>22.474494</v>
       </c>
       <c r="J6">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L6">
+        <v>-60</v>
+      </c>
+      <c r="M6">
+        <v>-40</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>22.474494</v>
+      </c>
+      <c r="P6">
         <v>2.2577542121616823</v>
-      </c>
-      <c r="M6">
-        <v>4.5155084243233645</v>
-      </c>
-      <c r="N6">
-        <v>6.7732626364850468</v>
-      </c>
-      <c r="O6">
-        <v>2.2577542121616823</v>
-      </c>
-      <c r="P6">
-        <v>22.473360000000003</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -895,28 +895,28 @@
         <v>12.228320939719493</v>
       </c>
       <c r="I7">
-        <v>4.4400000000000004</v>
+        <v>3.7007400000000001</v>
       </c>
       <c r="J7">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L7">
+        <v>-60</v>
+      </c>
+      <c r="M7">
+        <v>-40</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>3.7007400000000001</v>
+      </c>
+      <c r="P7">
         <v>2.1367296848367752</v>
-      </c>
-      <c r="M7">
-        <v>4.2734593696735503</v>
-      </c>
-      <c r="N7">
-        <v>6.4101890545103259</v>
-      </c>
-      <c r="O7">
-        <v>2.1367296848367752</v>
-      </c>
-      <c r="P7">
-        <v>3.7043999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -945,28 +945,28 @@
         <v>8.2996493711528831</v>
       </c>
       <c r="I8">
-        <v>4.7759999999999998</v>
+        <v>3.9807959999999998</v>
       </c>
       <c r="J8">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L8">
+        <v>-60</v>
+      </c>
+      <c r="M8">
+        <v>-40</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>3.9807959999999998</v>
+      </c>
+      <c r="P8">
         <v>3.3675065648772344</v>
-      </c>
-      <c r="M8">
-        <v>6.7350131297544689</v>
-      </c>
-      <c r="N8">
-        <v>10.102519694631702</v>
-      </c>
-      <c r="O8">
-        <v>3.3675065648772344</v>
-      </c>
-      <c r="P8">
-        <v>3.9780000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -995,28 +995,28 @@
         <v>45.577320398699342</v>
       </c>
       <c r="I9">
-        <v>23.795999999999996</v>
+        <v>19.833965999999997</v>
       </c>
       <c r="J9">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L9">
+        <v>-60</v>
+      </c>
+      <c r="M9">
+        <v>-40</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>19.833965999999997</v>
+      </c>
+      <c r="P9">
         <v>3.1770497211103974</v>
-      </c>
-      <c r="M9">
-        <v>6.3540994422207948</v>
-      </c>
-      <c r="N9">
-        <v>9.5311491633311931</v>
-      </c>
-      <c r="O9">
-        <v>3.1770497211103974</v>
-      </c>
-      <c r="P9">
-        <v>19.827360000000002</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1045,28 +1045,28 @@
         <v>1.796281342089298</v>
       </c>
       <c r="I10">
-        <v>0.94799999999999995</v>
+        <v>0.79015800000000003</v>
       </c>
       <c r="J10">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L10">
+        <v>-60</v>
+      </c>
+      <c r="M10">
+        <v>-40</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0.79015800000000003</v>
+      </c>
+      <c r="P10">
         <v>3.071691927986151</v>
-      </c>
-      <c r="M10">
-        <v>6.143383855972302</v>
-      </c>
-      <c r="N10">
-        <v>9.2150757839584525</v>
-      </c>
-      <c r="O10">
-        <v>3.071691927986151</v>
-      </c>
-      <c r="P10">
-        <v>0.79380000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1095,28 +1095,28 @@
         <v>52.731199907354139</v>
       </c>
       <c r="I11">
-        <v>6.1559999999999997</v>
+        <v>5.1310259999999994</v>
       </c>
       <c r="J11">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L11">
+        <v>-60</v>
+      </c>
+      <c r="M11">
+        <v>-40</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>5.1310259999999994</v>
+      </c>
+      <c r="P11">
         <v>0.7143478013034501</v>
-      </c>
-      <c r="M11">
-        <v>1.4286956026069002</v>
-      </c>
-      <c r="N11">
-        <v>2.1430434039103501</v>
-      </c>
-      <c r="O11">
-        <v>0.7143478013034501</v>
-      </c>
-      <c r="P11">
-        <v>5.1332399999999998</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1145,28 +1145,28 @@
         <v>13.724192033661508</v>
       </c>
       <c r="I12">
-        <v>0.80400000000000005</v>
+        <v>0.67013400000000001</v>
       </c>
       <c r="J12">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L12">
+        <v>-60</v>
+      </c>
+      <c r="M12">
+        <v>-40</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0.67013400000000001</v>
+      </c>
+      <c r="P12">
         <v>0.34469225101316964</v>
-      </c>
-      <c r="M12">
-        <v>0.68938450202633927</v>
-      </c>
-      <c r="N12">
-        <v>1.034076753039509</v>
-      </c>
-      <c r="O12">
-        <v>0.34469225101316964</v>
-      </c>
-      <c r="P12">
-        <v>0.67032000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1195,28 +1195,28 @@
         <v>155.46382238897644</v>
       </c>
       <c r="I13">
-        <v>19.943999999999999</v>
+        <v>16.623324</v>
       </c>
       <c r="J13">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L13">
+        <v>-60</v>
+      </c>
+      <c r="M13">
+        <v>-40</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>16.623324</v>
+      </c>
+      <c r="P13">
         <v>0.86496146254423367</v>
-      </c>
-      <c r="M13">
-        <v>1.7299229250884673</v>
-      </c>
-      <c r="N13">
-        <v>2.594884387632701</v>
-      </c>
-      <c r="O13">
-        <v>0.86496146254423367</v>
-      </c>
-      <c r="P13">
-        <v>16.616880000000002</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1245,28 +1245,28 @@
         <v>275.64439298550877</v>
       </c>
       <c r="I14">
-        <v>40.475999999999992</v>
+        <v>33.736745999999997</v>
       </c>
       <c r="J14">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L14">
+        <v>-60</v>
+      </c>
+      <c r="M14">
+        <v>-40</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>33.736745999999997</v>
+      </c>
+      <c r="P14">
         <v>1.0969792064708848</v>
-      </c>
-      <c r="M14">
-        <v>2.1939584129417695</v>
-      </c>
-      <c r="N14">
-        <v>3.2909376194126541</v>
-      </c>
-      <c r="O14">
-        <v>1.0969792064708848</v>
-      </c>
-      <c r="P14">
-        <v>33.727679999999999</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1295,28 +1295,28 @@
         <v>143.9305394189729</v>
       </c>
       <c r="I15">
-        <v>15.96</v>
+        <v>13.302660000000001</v>
       </c>
       <c r="J15">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L15">
+        <v>-60</v>
+      </c>
+      <c r="M15">
+        <v>-40</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>13.302660000000001</v>
+      </c>
+      <c r="P15">
         <v>0.73964612772368377</v>
-      </c>
-      <c r="M15">
-        <v>1.4792922554473675</v>
-      </c>
-      <c r="N15">
-        <v>2.2189383831710514</v>
-      </c>
-      <c r="O15">
-        <v>0.73964612772368377</v>
-      </c>
-      <c r="P15">
-        <v>13.300559999999999</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1345,28 +1345,28 @@
         <v>12.918316127211613</v>
       </c>
       <c r="I16">
-        <v>3.3479999999999999</v>
+        <v>2.7905579999999999</v>
       </c>
       <c r="J16">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L16">
+        <v>-60</v>
+      </c>
+      <c r="M16">
+        <v>-40</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>2.7905579999999999</v>
+      </c>
+      <c r="P16">
         <v>1.5229111097674977</v>
-      </c>
-      <c r="M16">
-        <v>3.0458222195349953</v>
-      </c>
-      <c r="N16">
-        <v>4.5687333293024928</v>
-      </c>
-      <c r="O16">
-        <v>1.5229111097674977</v>
-      </c>
-      <c r="P16">
-        <v>2.7871200000000003</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1395,28 +1395,28 @@
         <v>17.446018329557745</v>
       </c>
       <c r="I17">
-        <v>5.0760000000000005</v>
+        <v>4.2308460000000006</v>
       </c>
       <c r="J17">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L17">
+        <v>-60</v>
+      </c>
+      <c r="M17">
+        <v>-40</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>4.2308460000000006</v>
+      </c>
+      <c r="P17">
         <v>1.7213459986255004</v>
-      </c>
-      <c r="M17">
-        <v>3.4426919972510008</v>
-      </c>
-      <c r="N17">
-        <v>5.1640379958765017</v>
-      </c>
-      <c r="O17">
-        <v>1.7213459986255004</v>
-      </c>
-      <c r="P17">
-        <v>4.2336</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1445,28 +1445,28 @@
         <v>262.44237212644902</v>
       </c>
       <c r="I18">
-        <v>24.36</v>
+        <v>20.30406</v>
       </c>
       <c r="J18">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L18">
+        <v>-60</v>
+      </c>
+      <c r="M18">
+        <v>-40</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>20.30406</v>
+      </c>
+      <c r="P18">
         <v>0.68705617240035788</v>
-      </c>
-      <c r="M18">
-        <v>1.3741123448007158</v>
-      </c>
-      <c r="N18">
-        <v>2.0611685172010734</v>
-      </c>
-      <c r="O18">
-        <v>0.68705617240035788</v>
-      </c>
-      <c r="P18">
-        <v>20.303640000000001</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -1495,28 +1495,28 @@
         <v>94.321892452498446</v>
       </c>
       <c r="I19">
-        <v>39.431999999999995</v>
+        <v>32.866571999999998</v>
       </c>
       <c r="J19">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L19">
+        <v>-60</v>
+      </c>
+      <c r="M19">
+        <v>-40</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>32.866571999999998</v>
+      </c>
+      <c r="P19">
         <v>2.6669440174759429</v>
-      </c>
-      <c r="M19">
-        <v>5.3338880349518858</v>
-      </c>
-      <c r="N19">
-        <v>8.0008320524278282</v>
-      </c>
-      <c r="O19">
-        <v>2.6669440174759429</v>
-      </c>
-      <c r="P19">
-        <v>32.863320000000002</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1545,28 +1545,28 @@
         <v>61.405006859146269</v>
       </c>
       <c r="I20">
-        <v>25.152000000000001</v>
+        <v>20.964192000000001</v>
       </c>
       <c r="J20">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L20">
+        <v>-60</v>
+      </c>
+      <c r="M20">
+        <v>-40</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>20.964192000000001</v>
+      </c>
+      <c r="P20">
         <v>2.5324667381562982</v>
-      </c>
-      <c r="M20">
-        <v>5.0649334763125964</v>
-      </c>
-      <c r="N20">
-        <v>7.5974002144688946</v>
-      </c>
-      <c r="O20">
-        <v>2.5324667381562982</v>
-      </c>
-      <c r="P20">
-        <v>20.956320000000002</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1595,28 +1595,28 @@
         <v>194.78252319687192</v>
       </c>
       <c r="I21">
-        <v>15.491999999999999</v>
+        <v>12.912582</v>
       </c>
       <c r="J21">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L21">
+        <v>-60</v>
+      </c>
+      <c r="M21">
+        <v>-40</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>12.912582</v>
+      </c>
+      <c r="P21">
         <v>0.55396022614012119</v>
-      </c>
-      <c r="M21">
-        <v>1.1079204522802424</v>
-      </c>
-      <c r="N21">
-        <v>1.6618806784203635</v>
-      </c>
-      <c r="O21">
-        <v>0.55396022614012119</v>
-      </c>
-      <c r="P21">
-        <v>12.91248</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1645,28 +1645,28 @@
         <v>55.474687737252864</v>
       </c>
       <c r="I22">
-        <v>6.5039999999999996</v>
+        <v>5.4210839999999996</v>
       </c>
       <c r="J22">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L22">
+        <v>-60</v>
+      </c>
+      <c r="M22">
+        <v>-40</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>5.4210839999999996</v>
+      </c>
+      <c r="P22">
         <v>0.71754839180542296</v>
-      </c>
-      <c r="M22">
-        <v>1.4350967836108459</v>
-      </c>
-      <c r="N22">
-        <v>2.1526451754162688</v>
-      </c>
-      <c r="O22">
-        <v>0.71754839180542296</v>
-      </c>
-      <c r="P22">
-        <v>5.4154799999999996</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1695,28 +1695,28 @@
         <v>61.754422572539099</v>
       </c>
       <c r="I23">
-        <v>10.643999999999998</v>
+        <v>8.8717739999999985</v>
       </c>
       <c r="J23">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L23">
+        <v>-60</v>
+      </c>
+      <c r="M23">
+        <v>-40</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>8.8717739999999985</v>
+      </c>
+      <c r="P23">
         <v>1.0651425852178873</v>
-      </c>
-      <c r="M23">
-        <v>2.1302851704357746</v>
-      </c>
-      <c r="N23">
-        <v>3.1954277556536619</v>
-      </c>
-      <c r="O23">
-        <v>1.0651425852178873</v>
-      </c>
-      <c r="P23">
-        <v>8.8729200000000006</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -1745,28 +1745,28 @@
         <v>19.119107737690364</v>
       </c>
       <c r="I24">
-        <v>8.5559999999999992</v>
+        <v>7.1314259999999994</v>
       </c>
       <c r="J24">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L24">
+        <v>-60</v>
+      </c>
+      <c r="M24">
+        <v>-40</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>7.1314259999999994</v>
+      </c>
+      <c r="P24">
         <v>2.6500679504403895</v>
-      </c>
-      <c r="M24">
-        <v>5.3001359008807789</v>
-      </c>
-      <c r="N24">
-        <v>7.9502038513211684</v>
-      </c>
-      <c r="O24">
-        <v>2.6500679504403895</v>
-      </c>
-      <c r="P24">
-        <v>7.1265600000000004</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -1795,28 +1795,28 @@
         <v>208.51854107776924</v>
       </c>
       <c r="I25">
-        <v>24.071999999999999</v>
+        <v>20.064011999999998</v>
       </c>
       <c r="J25">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L25">
+        <v>-60</v>
+      </c>
+      <c r="M25">
+        <v>-40</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>20.064011999999998</v>
+      </c>
+      <c r="P25">
         <v>0.81547251145974264</v>
-      </c>
-      <c r="M25">
-        <v>1.6309450229194853</v>
-      </c>
-      <c r="N25">
-        <v>2.4464175343792278</v>
-      </c>
-      <c r="O25">
-        <v>0.81547251145974264</v>
-      </c>
-      <c r="P25">
-        <v>20.05668</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1845,28 +1845,28 @@
         <v>27.281384991573979</v>
       </c>
       <c r="I26">
-        <v>12.107999999999999</v>
+        <v>10.092017999999999</v>
       </c>
       <c r="J26">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L26">
+        <v>-60</v>
+      </c>
+      <c r="M26">
+        <v>-40</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>10.092017999999999</v>
+      </c>
+      <c r="P26">
         <v>2.6504213747458651</v>
-      </c>
-      <c r="M26">
-        <v>5.3008427494917303</v>
-      </c>
-      <c r="N26">
-        <v>7.9512641242375954</v>
-      </c>
-      <c r="O26">
-        <v>2.6504213747458651</v>
-      </c>
-      <c r="P26">
-        <v>10.09008</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -1895,28 +1895,28 @@
         <v>33.719044008434125</v>
       </c>
       <c r="I27">
-        <v>6.3119999999999994</v>
+        <v>5.2610519999999994</v>
       </c>
       <c r="J27">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L27">
+        <v>-60</v>
+      </c>
+      <c r="M27">
+        <v>-40</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>5.2610519999999994</v>
+      </c>
+      <c r="P27">
         <v>1.1237106940141237</v>
-      </c>
-      <c r="M27">
-        <v>2.2474213880282474</v>
-      </c>
-      <c r="N27">
-        <v>3.3711320820423714</v>
-      </c>
-      <c r="O27">
-        <v>1.1237106940141237</v>
-      </c>
-      <c r="P27">
-        <v>5.2567199999999996</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -1945,28 +1945,28 @@
         <v>49.448413422980799</v>
       </c>
       <c r="I28">
-        <v>6.48</v>
+        <v>5.4010800000000003</v>
       </c>
       <c r="J28">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L28">
+        <v>-60</v>
+      </c>
+      <c r="M28">
+        <v>-40</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>5.4010800000000003</v>
+      </c>
+      <c r="P28">
         <v>0.79941043356034458</v>
-      </c>
-      <c r="M28">
-        <v>1.5988208671206892</v>
-      </c>
-      <c r="N28">
-        <v>2.3982313006810339</v>
-      </c>
-      <c r="O28">
-        <v>0.79941043356034458</v>
-      </c>
-      <c r="P28">
-        <v>5.3978400000000004</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -1995,28 +1995,28 @@
         <v>102.49574354220591</v>
       </c>
       <c r="I29">
-        <v>35.58</v>
+        <v>29.655929999999998</v>
       </c>
       <c r="J29">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L29">
+        <v>-60</v>
+      </c>
+      <c r="M29">
+        <v>-40</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>29.655929999999998</v>
+      </c>
+      <c r="P29">
         <v>2.2304969312426666</v>
-      </c>
-      <c r="M29">
-        <v>4.4609938624853331</v>
-      </c>
-      <c r="N29">
-        <v>6.6914907937279997</v>
-      </c>
-      <c r="O29">
-        <v>2.2304969312426666</v>
-      </c>
-      <c r="P29">
-        <v>29.652840000000001</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -2045,28 +2045,28 @@
         <v>74.89225362970555</v>
       </c>
       <c r="I30">
-        <v>22.08</v>
+        <v>18.403679999999998</v>
       </c>
       <c r="J30">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L30">
+        <v>-60</v>
+      </c>
+      <c r="M30">
+        <v>-40</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>18.403679999999998</v>
+      </c>
+      <c r="P30">
         <v>1.8467493551032486</v>
-      </c>
-      <c r="M30">
-        <v>3.6934987102064971</v>
-      </c>
-      <c r="N30">
-        <v>5.5402480653097452</v>
-      </c>
-      <c r="O30">
-        <v>1.8467493551032486</v>
-      </c>
-      <c r="P30">
-        <v>18.398519999999998</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2095,28 +2095,28 @@
         <v>6.8797381415095664</v>
       </c>
       <c r="I31">
-        <v>3</v>
+        <v>2.5004999999999997</v>
       </c>
       <c r="J31">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L31">
+        <v>-60</v>
+      </c>
+      <c r="M31">
+        <v>-40</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>2.5004999999999997</v>
+      </c>
+      <c r="P31">
         <v>2.5480114419962745</v>
-      </c>
-      <c r="M31">
-        <v>5.096022883992549</v>
-      </c>
-      <c r="N31">
-        <v>7.644034325988823</v>
-      </c>
-      <c r="O31">
-        <v>2.5480114419962745</v>
-      </c>
-      <c r="P31">
-        <v>2.50488</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -2145,28 +2145,28 @@
         <v>27.48882571304776</v>
       </c>
       <c r="I32">
-        <v>9.8040000000000003</v>
+        <v>8.1716339999999992</v>
       </c>
       <c r="J32">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L32">
+        <v>-60</v>
+      </c>
+      <c r="M32">
+        <v>-40</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>8.1716339999999992</v>
+      </c>
+      <c r="P32">
         <v>2.132302591982465</v>
-      </c>
-      <c r="M32">
-        <v>4.2646051839649299</v>
-      </c>
-      <c r="N32">
-        <v>6.3969077759473949</v>
-      </c>
-      <c r="O32">
-        <v>2.132302591982465</v>
-      </c>
-      <c r="P32">
-        <v>8.1673200000000001</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -2195,28 +2195,28 @@
         <v>8.3880211812017578</v>
       </c>
       <c r="I33">
-        <v>3.0720000000000001</v>
+        <v>2.5605120000000001</v>
       </c>
       <c r="J33">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L33">
+        <v>-60</v>
+      </c>
+      <c r="M33">
+        <v>-40</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>2.5605120000000001</v>
+      </c>
+      <c r="P33">
         <v>2.1434788496065242</v>
-      </c>
-      <c r="M33">
-        <v>4.2869576992130485</v>
-      </c>
-      <c r="N33">
-        <v>6.4304365488195732</v>
-      </c>
-      <c r="O33">
-        <v>2.1434788496065242</v>
-      </c>
-      <c r="P33">
-        <v>2.5578000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -2245,28 +2245,28 @@
         <v>53.637397793021009</v>
       </c>
       <c r="I34">
-        <v>8.4</v>
+        <v>7.0014000000000003</v>
       </c>
       <c r="J34">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L34">
+        <v>-60</v>
+      </c>
+      <c r="M34">
+        <v>-40</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>7.0014000000000003</v>
+      </c>
+      <c r="P34">
         <v>0.95799035983516656</v>
-      </c>
-      <c r="M34">
-        <v>1.9159807196703331</v>
-      </c>
-      <c r="N34">
-        <v>2.8739710795054996</v>
-      </c>
-      <c r="O34">
-        <v>0.95799035983516656</v>
-      </c>
-      <c r="P34">
-        <v>7.0030800000000006</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -2295,28 +2295,28 @@
         <v>48.444436534230753</v>
       </c>
       <c r="I35">
-        <v>18.588000000000001</v>
+        <v>15.493098</v>
       </c>
       <c r="J35">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K35">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L35">
+        <v>-60</v>
+      </c>
+      <c r="M35">
+        <v>-40</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>15.493098</v>
+      </c>
+      <c r="P35">
         <v>2.3377851878514901</v>
-      </c>
-      <c r="M35">
-        <v>4.6755703757029803</v>
-      </c>
-      <c r="N35">
-        <v>7.0133555635544704</v>
-      </c>
-      <c r="O35">
-        <v>2.3377851878514901</v>
-      </c>
-      <c r="P35">
-        <v>15.487920000000001</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -2345,28 +2345,28 @@
         <v>21.401165215586502</v>
       </c>
       <c r="I36">
-        <v>7.6440000000000001</v>
+        <v>6.3712739999999997</v>
       </c>
       <c r="J36">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K36">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L36">
+        <v>-60</v>
+      </c>
+      <c r="M36">
+        <v>-40</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>6.3712739999999997</v>
+      </c>
+      <c r="P36">
         <v>2.1183837263904857</v>
-      </c>
-      <c r="M36">
-        <v>4.2367674527809713</v>
-      </c>
-      <c r="N36">
-        <v>6.3551511791714574</v>
-      </c>
-      <c r="O36">
-        <v>2.1183837263904857</v>
-      </c>
-      <c r="P36">
-        <v>6.3680399999999997</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -2395,28 +2395,28 @@
         <v>17.848949980499206</v>
       </c>
       <c r="I37">
-        <v>5.508</v>
+        <v>4.5909179999999994</v>
       </c>
       <c r="J37">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K37">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L37">
+        <v>-60</v>
+      </c>
+      <c r="M37">
+        <v>-40</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>4.5909179999999994</v>
+      </c>
+      <c r="P37">
         <v>1.8253803547622955</v>
-      </c>
-      <c r="M37">
-        <v>3.6507607095245911</v>
-      </c>
-      <c r="N37">
-        <v>5.4761410642868871</v>
-      </c>
-      <c r="O37">
-        <v>1.8253803547622955</v>
-      </c>
-      <c r="P37">
-        <v>4.5864000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -2445,28 +2445,28 @@
         <v>99.629801748397284</v>
       </c>
       <c r="I38">
-        <v>32.112000000000002</v>
+        <v>26.765352</v>
       </c>
       <c r="J38">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L38">
+        <v>-60</v>
+      </c>
+      <c r="M38">
+        <v>-40</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>26.765352</v>
+      </c>
+      <c r="P38">
         <v>2.0673544330144757</v>
-      </c>
-      <c r="M38">
-        <v>4.1347088660289515</v>
-      </c>
-      <c r="N38">
-        <v>6.2020632990434272</v>
-      </c>
-      <c r="O38">
-        <v>2.0673544330144757</v>
-      </c>
-      <c r="P38">
-        <v>26.759879999999999</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -2495,28 +2495,28 @@
         <v>39.581326107542793</v>
       </c>
       <c r="I39">
-        <v>13.127999999999998</v>
+        <v>10.942188</v>
       </c>
       <c r="J39">
-        <v>661.66300000000001</v>
+        <v>921.04403669765156</v>
       </c>
       <c r="K39">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="L39">
+        <v>-60</v>
+      </c>
+      <c r="M39">
+        <v>-40</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>10.942188</v>
+      </c>
+      <c r="P39">
         <v>2.004574802018523</v>
-      </c>
-      <c r="M39">
-        <v>4.009149604037046</v>
-      </c>
-      <c r="N39">
-        <v>6.0137244060555695</v>
-      </c>
-      <c r="O39">
-        <v>2.004574802018523</v>
-      </c>
-      <c r="P39">
-        <v>10.9368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimizing for Faster Processing
- Stored project parameters in the CanvasModel, allowing for parameters such as SimEndTime and PhysicsTimeStep to be modified
- Added a Body subclass for bone objects, allowing for better storage of bone-related information such as COM location and mass
- FullLeg will now collect and store some information in Body objects
- FullLeg: Optimized muscle moment arm code dramatically
- FullLeg: Added a compute_gravity_moment_arm function to allow for finding torques due to body weight
- indivProjectBuilder: builds a project with direct MN stimulation instead of synergy stimulation
- sumsinesFit: Increased optimization function tolerance for faster curve fitting
- temp_wthresh: Implemented synergy sorting to maintain synergy order while plotting iteratively
</commit_message>
<xml_diff>
--- a/ParameterCalculation/MuscleParameters_20190513.xlsx
+++ b/ParameterCalculation/MuscleParameters_20190513.xlsx
@@ -651,7 +651,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K2">
-        <v>-1E-3</v>
+        <v>-2.1984395999999999</v>
       </c>
       <c r="L2">
         <v>-60</v>
@@ -701,7 +701,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K3">
-        <v>-1E-3</v>
+        <v>-0.18703740000000002</v>
       </c>
       <c r="L3">
         <v>-60</v>
@@ -751,7 +751,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K4">
-        <v>-1E-3</v>
+        <v>-0.54310860000000005</v>
       </c>
       <c r="L4">
         <v>-60</v>
@@ -801,7 +801,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K5">
-        <v>-1E-3</v>
+        <v>-0.61012200000000005</v>
       </c>
       <c r="L5">
         <v>-60</v>
@@ -851,7 +851,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K6">
-        <v>-1E-3</v>
+        <v>-2.2474493999999998</v>
       </c>
       <c r="L6">
         <v>-60</v>
@@ -901,7 +901,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K7">
-        <v>-1E-3</v>
+        <v>-0.37007400000000001</v>
       </c>
       <c r="L7">
         <v>-60</v>
@@ -951,7 +951,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K8">
-        <v>-1E-3</v>
+        <v>-0.39807960000000003</v>
       </c>
       <c r="L8">
         <v>-60</v>
@@ -1001,7 +1001,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K9">
-        <v>-1E-3</v>
+        <v>-1.9833965999999998</v>
       </c>
       <c r="L9">
         <v>-60</v>
@@ -1051,7 +1051,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K10">
-        <v>-1E-3</v>
+        <v>-7.9015799999999997E-2</v>
       </c>
       <c r="L10">
         <v>-60</v>
@@ -1101,7 +1101,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K11">
-        <v>-1E-3</v>
+        <v>-0.51310260000000008</v>
       </c>
       <c r="L11">
         <v>-60</v>
@@ -1151,7 +1151,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K12">
-        <v>-1E-3</v>
+        <v>-6.7013400000000001E-2</v>
       </c>
       <c r="L12">
         <v>-60</v>
@@ -1201,7 +1201,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K13">
-        <v>-1E-3</v>
+        <v>-1.6623324000000002</v>
       </c>
       <c r="L13">
         <v>-60</v>
@@ -1251,7 +1251,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K14">
-        <v>-1E-3</v>
+        <v>-3.3736745999999997</v>
       </c>
       <c r="L14">
         <v>-60</v>
@@ -1301,7 +1301,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K15">
-        <v>-1E-3</v>
+        <v>-1.3302660000000002</v>
       </c>
       <c r="L15">
         <v>-60</v>
@@ -1351,7 +1351,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K16">
-        <v>-1E-3</v>
+        <v>-0.27905580000000002</v>
       </c>
       <c r="L16">
         <v>-60</v>
@@ -1401,7 +1401,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K17">
-        <v>-1E-3</v>
+        <v>-0.42308460000000009</v>
       </c>
       <c r="L17">
         <v>-60</v>
@@ -1451,7 +1451,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K18">
-        <v>-1E-3</v>
+        <v>-2.0304060000000002</v>
       </c>
       <c r="L18">
         <v>-60</v>
@@ -1501,7 +1501,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K19">
-        <v>-1E-3</v>
+        <v>-3.2866572000000001</v>
       </c>
       <c r="L19">
         <v>-60</v>
@@ -1551,7 +1551,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K20">
-        <v>-1E-3</v>
+        <v>-2.0964192000000001</v>
       </c>
       <c r="L20">
         <v>-60</v>
@@ -1601,7 +1601,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K21">
-        <v>-1E-3</v>
+        <v>-1.2912582000000001</v>
       </c>
       <c r="L21">
         <v>-60</v>
@@ -1651,7 +1651,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K22">
-        <v>-1E-3</v>
+        <v>-0.54210840000000005</v>
       </c>
       <c r="L22">
         <v>-60</v>
@@ -1701,7 +1701,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K23">
-        <v>-1E-3</v>
+        <v>-0.8871774</v>
       </c>
       <c r="L23">
         <v>-60</v>
@@ -1751,7 +1751,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K24">
-        <v>-1E-3</v>
+        <v>-0.71314260000000007</v>
       </c>
       <c r="L24">
         <v>-60</v>
@@ -1801,7 +1801,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K25">
-        <v>-1E-3</v>
+        <v>-2.0064012</v>
       </c>
       <c r="L25">
         <v>-60</v>
@@ -1851,7 +1851,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K26">
-        <v>-1E-3</v>
+        <v>-1.0092018</v>
       </c>
       <c r="L26">
         <v>-60</v>
@@ -1901,7 +1901,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K27">
-        <v>-1E-3</v>
+        <v>-0.52610519999999994</v>
       </c>
       <c r="L27">
         <v>-60</v>
@@ -1951,7 +1951,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K28">
-        <v>-1E-3</v>
+        <v>-0.54010800000000003</v>
       </c>
       <c r="L28">
         <v>-60</v>
@@ -2001,7 +2001,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K29">
-        <v>-1E-3</v>
+        <v>-2.9655930000000001</v>
       </c>
       <c r="L29">
         <v>-60</v>
@@ -2051,7 +2051,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K30">
-        <v>-1E-3</v>
+        <v>-1.840368</v>
       </c>
       <c r="L30">
         <v>-60</v>
@@ -2101,7 +2101,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K31">
-        <v>-1E-3</v>
+        <v>-0.25005000000000005</v>
       </c>
       <c r="L31">
         <v>-60</v>
@@ -2151,7 +2151,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K32">
-        <v>-1E-3</v>
+        <v>-0.81716339999999998</v>
       </c>
       <c r="L32">
         <v>-60</v>
@@ -2201,7 +2201,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K33">
-        <v>-1E-3</v>
+        <v>-0.25605120000000003</v>
       </c>
       <c r="L33">
         <v>-60</v>
@@ -2251,7 +2251,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K34">
-        <v>-1E-3</v>
+        <v>-0.70013999999999998</v>
       </c>
       <c r="L34">
         <v>-60</v>
@@ -2301,7 +2301,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K35">
-        <v>-1E-3</v>
+        <v>-1.5493098000000001</v>
       </c>
       <c r="L35">
         <v>-60</v>
@@ -2351,7 +2351,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K36">
-        <v>-1E-3</v>
+        <v>-0.63712740000000001</v>
       </c>
       <c r="L36">
         <v>-60</v>
@@ -2401,7 +2401,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K37">
-        <v>-1E-3</v>
+        <v>-0.45909179999999999</v>
       </c>
       <c r="L37">
         <v>-60</v>
@@ -2451,7 +2451,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K38">
-        <v>-1E-3</v>
+        <v>-2.6765352000000004</v>
       </c>
       <c r="L38">
         <v>-60</v>
@@ -2501,7 +2501,7 @@
         <v>921.04403669765156</v>
       </c>
       <c r="K39">
-        <v>-1E-3</v>
+        <v>-1.0942187999999999</v>
       </c>
       <c r="L39">
         <v>-60</v>

</xml_diff>

<commit_message>
Examining Animatlab's Tension Function in the Context of Oscillations
- Created reduced version of muscle models and changes associated files to accommodate accordingly
- CanvasModel: now checks for existing stimuli and keeps motor stimuli while eliminating any electrical stimuli
- sum_of_sines_maker: dug into equation generator edge cases and made the program more reliable for the number of input sines waves
- passivePropSolver: modified selection criteria since one success criteria was redundant
- FullLeg: changed passive tension equation to reflect Animatlab's actual behavior. Output now matches simulation results, minus the oscillations
- FullLeg: changes force optimizer lower bound, simplifying it to the passive muscle tension
</commit_message>
<xml_diff>
--- a/ParameterCalculation/MuscleParameters_20190513.xlsx
+++ b/ParameterCalculation/MuscleParameters_20190513.xlsx
@@ -152,22 +152,22 @@
     <t>vastus medialis</t>
   </si>
   <si>
+    <t>extensor digitorum longus</t>
+  </si>
+  <si>
     <t>Ks</t>
   </si>
   <si>
     <t>Kp</t>
   </si>
   <si>
+    <t>Stmax</t>
+  </si>
+  <si>
+    <t>Steepness</t>
+  </si>
+  <si>
     <t>Yoff</t>
-  </si>
-  <si>
-    <t>extensor digitorum longus</t>
-  </si>
-  <si>
-    <t>Stmax</t>
-  </si>
-  <si>
-    <t>Steepness</t>
   </si>
   <si>
     <t>STLowerLimit</t>
@@ -601,19 +601,19 @@
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>48</v>
@@ -663,19 +663,19 @@
         <v>12.210800000000003</v>
       </c>
       <c r="G2">
-        <v>624.06144759882136</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H2">
-        <v>66.64026880280457</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I2">
-        <v>13.50473195312202</v>
+        <v>13.431000000000003</v>
       </c>
       <c r="J2">
-        <v>1469.0678455660432</v>
+        <v>1765.2638143334184</v>
       </c>
       <c r="K2">
-        <v>-1.6785929723100883E-10</v>
+        <v>-2.0333978062304618E-10</v>
       </c>
       <c r="L2">
         <v>-60</v>
@@ -687,7 +687,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>13.50473195312202</v>
+        <v>13.431000000000003</v>
       </c>
       <c r="P2">
         <v>1.0740679384557621</v>
@@ -725,19 +725,19 @@
         <v>1.0388000000000002</v>
       </c>
       <c r="G3">
-        <v>479.11626256008503</v>
+        <v>365.81617683817126</v>
       </c>
       <c r="H3">
-        <v>72.827341320165303</v>
+        <v>76.350464084881338</v>
       </c>
       <c r="I3">
-        <v>1.1445269692652769</v>
+        <v>1.1440000000000001</v>
       </c>
       <c r="J3">
-        <v>970.59278279873809</v>
+        <v>970.5927828387305</v>
       </c>
       <c r="K3">
-        <v>1.0419807334153966E-8</v>
+        <v>1.0419807356569846E-8</v>
       </c>
       <c r="L3">
         <v>-60</v>
@@ -749,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1.1445269692652769</v>
+        <v>1.1440000000000001</v>
       </c>
       <c r="P3">
         <v>0.6819514577231951</v>
@@ -787,19 +787,19 @@
         <v>3.0184000000000006</v>
       </c>
       <c r="G4">
-        <v>546.80582725025954</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H4">
-        <v>70.109414618967733</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I4">
-        <v>3.3270380344277748</v>
+        <v>3.3220000000000005</v>
       </c>
       <c r="J4">
-        <v>970.5927908791374</v>
+        <v>970.59279085163746</v>
       </c>
       <c r="K4">
-        <v>1.0419807500579E-8</v>
+        <v>1.0419807461005621E-8</v>
       </c>
       <c r="L4">
         <v>-60</v>
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>3.3270380344277748</v>
+        <v>3.3220000000000005</v>
       </c>
       <c r="P4">
         <v>1.4754747575459182</v>
@@ -849,19 +849,19 @@
         <v>3.3908000000000005</v>
       </c>
       <c r="G5">
-        <v>430.20766894478544</v>
+        <v>365.81617683817126</v>
       </c>
       <c r="H5">
-        <v>83.138039175595836</v>
+        <v>76.350464084881338</v>
       </c>
       <c r="I5">
-        <v>3.7315070402806132</v>
+        <v>3.7290000000000005</v>
       </c>
       <c r="J5">
-        <v>976.02421003177699</v>
+        <v>1074.905534196183</v>
       </c>
       <c r="K5">
-        <v>5.4454271825462511E-10</v>
+        <v>1.4681972756055362E-9</v>
       </c>
       <c r="L5">
         <v>-60</v>
@@ -873,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>3.7315070402806132</v>
+        <v>3.7290000000000005</v>
       </c>
       <c r="P5">
         <v>2.6026604179888015</v>
@@ -911,19 +911,19 @@
         <v>12.485200000000003</v>
       </c>
       <c r="G6">
-        <v>624.06145641878834</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H6">
-        <v>66.640852574175881</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I6">
-        <v>13.784375049570835</v>
+        <v>13.739000000000001</v>
       </c>
       <c r="J6">
-        <v>2633.999595108899</v>
+        <v>1766.8955992803633</v>
       </c>
       <c r="K6">
-        <v>3.5377981045071807E-10</v>
+        <v>-1.3013249591551181E-11</v>
       </c>
       <c r="L6">
         <v>-60</v>
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>13.784375049570835</v>
+        <v>13.739000000000001</v>
       </c>
       <c r="P6">
         <v>2.2577542121616823</v>
@@ -973,19 +973,19 @@
         <v>2.0580000000000003</v>
       </c>
       <c r="G7">
-        <v>301.24647162666298</v>
+        <v>44.454092278238491</v>
       </c>
       <c r="H7">
-        <v>51.859359855900365</v>
+        <v>75.493326723117917</v>
       </c>
       <c r="I7">
-        <v>2.2804994932434184</v>
+        <v>2.2660000000000005</v>
       </c>
       <c r="J7">
-        <v>970.5927860037192</v>
+        <v>970.59278599053619</v>
       </c>
       <c r="K7">
-        <v>1.0419795655236585E-8</v>
+        <v>1.0419807395113233E-8</v>
       </c>
       <c r="L7">
         <v>-60</v>
@@ -997,7 +997,7 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>2.2804994932434184</v>
+        <v>2.2660000000000005</v>
       </c>
       <c r="P7">
         <v>2.1367296848367752</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3">
         <v>146</v>
@@ -1035,19 +1035,19 @@
         <v>2.21</v>
       </c>
       <c r="G8">
-        <v>136.55334316123088</v>
+        <v>199.86282285745204</v>
       </c>
       <c r="H8">
-        <v>15.639143309871914</v>
+        <v>40.695483713890681</v>
       </c>
       <c r="I8">
-        <v>2.4352824993449973</v>
+        <v>2.431</v>
       </c>
       <c r="J8">
-        <v>970.59278660516441</v>
+        <v>970.59278662901943</v>
       </c>
       <c r="K8">
-        <v>1.0419807287370643E-8</v>
+        <v>1.041980746068036E-8</v>
       </c>
       <c r="L8">
         <v>-60</v>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>2.4352824993449973</v>
+        <v>2.431</v>
       </c>
       <c r="P8">
         <v>3.3675065648772344</v>
@@ -1097,19 +1097,19 @@
         <v>11.015200000000002</v>
       </c>
       <c r="G9">
-        <v>721.22856201638797</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H9">
-        <v>85.54561116851761</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I9">
-        <v>12.178728837327125</v>
+        <v>12.122</v>
       </c>
       <c r="J9">
-        <v>1375.9317567338651</v>
+        <v>2712.2260469545163</v>
       </c>
       <c r="K9">
-        <v>2.7842126223245292E-10</v>
+        <v>9.8994955296440991E-11</v>
       </c>
       <c r="L9">
         <v>-60</v>
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>12.178728837327125</v>
+        <v>12.122</v>
       </c>
       <c r="P9">
         <v>3.1770497211103974</v>
@@ -1159,19 +1159,19 @@
         <v>0.44100000000000006</v>
       </c>
       <c r="G10">
-        <v>30.542745797368521</v>
+        <v>21.555887203496994</v>
       </c>
       <c r="H10">
-        <v>25.182373394580889</v>
+        <v>55.984070587250969</v>
       </c>
       <c r="I10">
-        <v>0.50980500315157429</v>
+        <v>0.48400000000000004</v>
       </c>
       <c r="J10">
-        <v>970.59278197471656</v>
+        <v>970.59278195359286</v>
       </c>
       <c r="K10">
-        <v>1.0419807385897515E-8</v>
+        <v>1.0419807394977708E-8</v>
       </c>
       <c r="L10">
         <v>-60</v>
@@ -1183,7 +1183,7 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>0.50980500315157429</v>
+        <v>0.48400000000000004</v>
       </c>
       <c r="P10">
         <v>3.071691927986151</v>
@@ -1221,19 +1221,19 @@
         <v>2.8518000000000003</v>
       </c>
       <c r="G11">
-        <v>624.0601556143547</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H11">
-        <v>66.652242268037327</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I11">
-        <v>3.1363286422203025</v>
+        <v>3.1350000000000002</v>
       </c>
       <c r="J11">
-        <v>1059.9762847460215</v>
+        <v>1059.9398293869169</v>
       </c>
       <c r="K11">
-        <v>6.7217209733866137E-10</v>
+        <v>1.0122742547722417E-9</v>
       </c>
       <c r="L11">
         <v>-60</v>
@@ -1245,7 +1245,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>3.1363286422203025</v>
+        <v>3.1350000000000002</v>
       </c>
       <c r="P11">
         <v>0.7143478013034501</v>
@@ -1283,19 +1283,19 @@
         <v>0.37240000000000006</v>
       </c>
       <c r="G12">
-        <v>136.55314388605373</v>
+        <v>44.454092278238491</v>
       </c>
       <c r="H12">
-        <v>15.640443523825214</v>
+        <v>75.493326723117917</v>
       </c>
       <c r="I12">
-        <v>0.41060730490529451</v>
+        <v>0.40700000000000003</v>
       </c>
       <c r="J12">
-        <v>970.59278189950487</v>
+        <v>970.59278189707743</v>
       </c>
       <c r="K12">
-        <v>1.0419807383702006E-8</v>
+        <v>1.0419807379283882E-8</v>
       </c>
       <c r="L12">
         <v>-60</v>
@@ -1307,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>0.41060730490529451</v>
+        <v>0.40700000000000003</v>
       </c>
       <c r="P12">
         <v>0.34469225101316964</v>
@@ -1345,19 +1345,19 @@
         <v>9.231600000000002</v>
       </c>
       <c r="G13">
-        <v>624.06086369396542</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H13">
-        <v>66.645663119495822</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I13">
-        <v>10.207755956379376</v>
+        <v>10.153</v>
       </c>
       <c r="J13">
-        <v>1642.1828665218409</v>
+        <v>1444.711873773193</v>
       </c>
       <c r="K13">
-        <v>-2.5992357459320412E-10</v>
+        <v>-2.1138595844171893E-10</v>
       </c>
       <c r="L13">
         <v>-60</v>
@@ -1369,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>10.207755956379376</v>
+        <v>10.153</v>
       </c>
       <c r="P13">
         <v>0.86496146254423367</v>
@@ -1407,19 +1407,19 @@
         <v>18.737600000000004</v>
       </c>
       <c r="G14">
-        <v>624.0633110204999</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H14">
-        <v>66.622830904781537</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I14">
-        <v>20.734822094142675</v>
+        <v>20.614000000000001</v>
       </c>
       <c r="J14">
-        <v>1621.4804760413581</v>
+        <v>1323.6415507499746</v>
       </c>
       <c r="K14">
-        <v>-8.0513484441093456E-10</v>
+        <v>-4.9539255537442846E-9</v>
       </c>
       <c r="L14">
         <v>-60</v>
@@ -1431,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>20.734822094142675</v>
+        <v>20.614000000000001</v>
       </c>
       <c r="P14">
         <v>1.0969792064708848</v>
@@ -1469,19 +1469,19 @@
         <v>7.3892000000000007</v>
       </c>
       <c r="G15">
-        <v>624.0605843130428</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H15">
-        <v>66.6482430924749</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I15">
-        <v>8.1719055214805874</v>
+        <v>8.1289999999999996</v>
       </c>
       <c r="J15">
-        <v>1440.9893293246369</v>
+        <v>1042.8159564824132</v>
       </c>
       <c r="K15">
-        <v>-1.2747448716563565E-9</v>
+        <v>1.1185604763214426E-9</v>
       </c>
       <c r="L15">
         <v>-60</v>
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>8.1719055214805874</v>
+        <v>8.1289999999999996</v>
       </c>
       <c r="P15">
         <v>0.73964612772368377</v>
@@ -1531,19 +1531,19 @@
         <v>1.5484000000000002</v>
       </c>
       <c r="G16">
-        <v>136.55325114784173</v>
+        <v>44.454092278238491</v>
       </c>
       <c r="H16">
-        <v>15.63960486533932</v>
+        <v>75.493326723117917</v>
       </c>
       <c r="I16">
-        <v>1.71935213174331</v>
+        <v>1.7050000000000003</v>
       </c>
       <c r="J16">
-        <v>970.59278419584496</v>
+        <v>970.59278415537017</v>
       </c>
       <c r="K16">
-        <v>1.0419807387957499E-8</v>
+        <v>1.0419807411349161E-8</v>
       </c>
       <c r="L16">
         <v>-60</v>
@@ -1555,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>1.71935213174331</v>
+        <v>1.7050000000000003</v>
       </c>
       <c r="P16">
         <v>1.5229111097674977</v>
@@ -1593,19 +1593,19 @@
         <v>2.3520000000000003</v>
       </c>
       <c r="G17">
-        <v>408.71996257465514</v>
+        <v>365.81617683817126</v>
       </c>
       <c r="H17">
-        <v>62.797097703519825</v>
+        <v>76.350464084881338</v>
       </c>
       <c r="I17">
-        <v>2.5990357302233087</v>
+        <v>2.5850000000000004</v>
       </c>
       <c r="J17">
-        <v>970.59278732522307</v>
+        <v>970.59278726535365</v>
       </c>
       <c r="K17">
-        <v>1.0419807412677309E-8</v>
+        <v>1.041980744083946E-8</v>
       </c>
       <c r="L17">
         <v>-60</v>
@@ -1617,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="O17">
-        <v>2.5990357302233087</v>
+        <v>2.5850000000000004</v>
       </c>
       <c r="P17">
         <v>1.7213459986255004</v>
@@ -1655,19 +1655,19 @@
         <v>11.279800000000002</v>
       </c>
       <c r="G18">
-        <v>624.06125556099209</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H18">
-        <v>66.641945268650232</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I18">
-        <v>12.480535178238817</v>
+        <v>12.407999999999999</v>
       </c>
       <c r="J18">
-        <v>1378.0419026995967</v>
+        <v>1876.3450388558454</v>
       </c>
       <c r="K18">
-        <v>-3.6775026391110021E-10</v>
+        <v>-1.8048018280388312E-10</v>
       </c>
       <c r="L18">
         <v>-60</v>
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>12.480535178238817</v>
+        <v>12.407999999999999</v>
       </c>
       <c r="P18">
         <v>0.68705617240035788</v>
@@ -1717,19 +1717,19 @@
         <v>18.257400000000004</v>
       </c>
       <c r="G19">
-        <v>624.0630703971874</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H19">
-        <v>66.626106947123446</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I19">
-        <v>20.173983828809817</v>
+        <v>20.086000000000002</v>
       </c>
       <c r="J19">
-        <v>2652.0708589746887</v>
+        <v>1799.818113478547</v>
       </c>
       <c r="K19">
-        <v>4.5113890830963787E-10</v>
+        <v>-1.7398939151253088E-10</v>
       </c>
       <c r="L19">
         <v>-60</v>
@@ -1741,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <v>20.173983828809817</v>
+        <v>20.086000000000002</v>
       </c>
       <c r="P19">
         <v>2.6669440174759429</v>
@@ -1779,19 +1779,19 @@
         <v>11.642400000000002</v>
       </c>
       <c r="G20">
-        <v>624.06124828253485</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H20">
-        <v>66.642994665659344</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I20">
-        <v>12.829683746567945</v>
+        <v>12.804000000000002</v>
       </c>
       <c r="J20">
-        <v>2647.3773929331401</v>
+        <v>1661.7803694415495</v>
       </c>
       <c r="K20">
-        <v>2.808799407728362E-10</v>
+        <v>3.0012552151959176E-10</v>
       </c>
       <c r="L20">
         <v>-60</v>
@@ -1803,7 +1803,7 @@
         <v>0</v>
       </c>
       <c r="O20">
-        <v>12.829683746567945</v>
+        <v>12.804000000000002</v>
       </c>
       <c r="P20">
         <v>2.5324667381562982</v>
@@ -1841,19 +1841,19 @@
         <v>7.1736000000000013</v>
       </c>
       <c r="G21">
-        <v>624.06055817390131</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H21">
-        <v>66.648445744349019</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I21">
-        <v>7.931490318665019</v>
+        <v>7.8870000000000005</v>
       </c>
       <c r="J21">
-        <v>1139.8391418001941</v>
+        <v>1338.2590390464227</v>
       </c>
       <c r="K21">
-        <v>2.3523067481785238E-10</v>
+        <v>-1.0980806543315517E-9</v>
       </c>
       <c r="L21">
         <v>-60</v>
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="O21">
-        <v>7.931490318665019</v>
+        <v>7.8870000000000005</v>
       </c>
       <c r="P21">
         <v>0.55396022614012119</v>
@@ -1903,19 +1903,19 @@
         <v>3.0086000000000004</v>
       </c>
       <c r="G22">
-        <v>624.06016417754768</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H22">
-        <v>66.65216415946702</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I22">
-        <v>3.3141507381831028</v>
+        <v>3.3109999999999999</v>
       </c>
       <c r="J22">
-        <v>970.59279080871295</v>
+        <v>970.5927907915642</v>
       </c>
       <c r="K22">
-        <v>1.041980749811244E-8</v>
+        <v>1.0419807369227907E-8</v>
       </c>
       <c r="L22">
         <v>-60</v>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="O22">
-        <v>3.3141507381831028</v>
+        <v>3.3109999999999999</v>
       </c>
       <c r="P22">
         <v>0.71754839180542296</v>
@@ -1965,19 +1965,19 @@
         <v>4.9294000000000011</v>
       </c>
       <c r="G23">
-        <v>624.06029595564496</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H23">
-        <v>66.651034363079205</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I23">
-        <v>5.4335059158519297</v>
+        <v>5.423</v>
       </c>
       <c r="J23">
-        <v>1008.2404246480997</v>
+        <v>1305.9138355421981</v>
       </c>
       <c r="K23">
-        <v>8.1861017627553006E-10</v>
+        <v>-3.0927586036675757E-10</v>
       </c>
       <c r="L23">
         <v>-60</v>
@@ -1989,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="O23">
-        <v>5.4335059158519297</v>
+        <v>5.423</v>
       </c>
       <c r="P23">
         <v>1.0651425852178873</v>
@@ -2027,19 +2027,19 @@
         <v>3.9592000000000005</v>
       </c>
       <c r="G24">
-        <v>470.92379486522304</v>
+        <v>365.81617683817126</v>
       </c>
       <c r="H24">
-        <v>97.29750580148027</v>
+        <v>76.350464084881338</v>
       </c>
       <c r="I24">
-        <v>4.4013311675828852</v>
+        <v>4.3559999999999999</v>
       </c>
       <c r="J24">
-        <v>990.19262572854973</v>
+        <v>989.30497722942198</v>
       </c>
       <c r="K24">
-        <v>1.1256947676461478E-9</v>
+        <v>-5.7586706766882303E-11</v>
       </c>
       <c r="L24">
         <v>-60</v>
@@ -2051,7 +2051,7 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <v>4.4013311675828852</v>
+        <v>4.3559999999999999</v>
       </c>
       <c r="P24">
         <v>2.6500679504403895</v>
@@ -2089,19 +2089,19 @@
         <v>11.142600000000002</v>
       </c>
       <c r="G25">
-        <v>624.06122388880704</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H25">
-        <v>66.642276408803042</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I25">
-        <v>12.323839197854086</v>
+        <v>12.254000000000001</v>
       </c>
       <c r="J25">
-        <v>2250.0528536692518</v>
+        <v>1363.0300503908536</v>
       </c>
       <c r="K25">
-        <v>1.0971613754949344E-10</v>
+        <v>2.8670327384551484E-10</v>
       </c>
       <c r="L25">
         <v>-60</v>
@@ -2113,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>12.323839197854086</v>
+        <v>12.254000000000001</v>
       </c>
       <c r="P25">
         <v>0.81547251145974264</v>
@@ -2151,19 +2151,19 @@
         <v>5.6056000000000008</v>
       </c>
       <c r="G26">
-        <v>424.16720206189478</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H26">
-        <v>48.965818883807017</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I26">
-        <v>6.1907096274444484</v>
+        <v>6.1710000000000012</v>
       </c>
       <c r="J26">
-        <v>1019.4167367615596</v>
+        <v>1019.1434104915377</v>
       </c>
       <c r="K26">
-        <v>-4.6775494021114038E-10</v>
+        <v>2.7320588799080375E-12</v>
       </c>
       <c r="L26">
         <v>-60</v>
@@ -2175,7 +2175,7 @@
         <v>0</v>
       </c>
       <c r="O26">
-        <v>6.1907096274444484</v>
+        <v>6.1710000000000012</v>
       </c>
       <c r="P26">
         <v>2.6504213747458651</v>
@@ -2213,19 +2213,19 @@
         <v>2.9204000000000003</v>
       </c>
       <c r="G27">
-        <v>617.66646949267204</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H27">
-        <v>73.024428565466849</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I27">
-        <v>3.2128058482835096</v>
+        <v>3.2120000000000002</v>
       </c>
       <c r="J27">
-        <v>970.59279026376703</v>
+        <v>970.59279025946125</v>
       </c>
       <c r="K27">
-        <v>1.0419807366381876E-8</v>
+        <v>1.0419807318378825E-8</v>
       </c>
       <c r="L27">
         <v>-60</v>
@@ -2237,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>3.2128058482835096</v>
+        <v>3.2120000000000002</v>
       </c>
       <c r="P27">
         <v>1.1237106940141237</v>
@@ -2275,19 +2275,19 @@
         <v>2.9988000000000006</v>
       </c>
       <c r="G28">
-        <v>721.22757955285078</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H28">
-        <v>85.551747966297384</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I28">
-        <v>3.3206461015993676</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="J28">
-        <v>1064.9028221033132</v>
+        <v>970.59279073154835</v>
       </c>
       <c r="K28">
-        <v>-8.3052139007462734E-10</v>
+        <v>1.0419807462387978E-8</v>
       </c>
       <c r="L28">
         <v>-60</v>
@@ -2299,7 +2299,7 @@
         <v>0</v>
       </c>
       <c r="O28">
-        <v>3.3206461015993676</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="P28">
         <v>0.79941043356034458</v>
@@ -2337,19 +2337,19 @@
         <v>10.221400000000001</v>
       </c>
       <c r="G29">
-        <v>624.06252386543122</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H29">
-        <v>66.63085656376542</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I29">
-        <v>18.200430466460837</v>
+        <v>11.242000000000001</v>
       </c>
       <c r="J29">
-        <v>1791.1619501199848</v>
+        <v>1355.7248731180293</v>
       </c>
       <c r="K29">
-        <v>-2.8412443779677339E-10</v>
+        <v>-9.7866131654512724E-11</v>
       </c>
       <c r="L29">
         <v>-60</v>
@@ -2361,22 +2361,22 @@
         <v>0</v>
       </c>
       <c r="O29">
-        <v>18.200430466460837</v>
+        <v>11.242000000000001</v>
       </c>
       <c r="P29">
-        <v>2.2304969312426666</v>
+        <v>1.8467493551032486</v>
       </c>
       <c r="Q29">
-        <v>4.4609938624853331</v>
+        <v>3.6934987102064971</v>
       </c>
       <c r="R29">
-        <v>6.6914907937279997</v>
+        <v>5.5402480653097452</v>
       </c>
       <c r="S29">
-        <v>2.2304969312426666</v>
+        <v>1.8467493551032486</v>
       </c>
       <c r="T29">
-        <v>16.473800000000001</v>
+        <v>10.221399999999999</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -2399,19 +2399,19 @@
         <v>1.3916000000000002</v>
       </c>
       <c r="G30">
-        <v>624.06100379914483</v>
+        <v>111.70574419320344</v>
       </c>
       <c r="H30">
-        <v>66.644799263288036</v>
+        <v>13.629254893829867</v>
       </c>
       <c r="I30">
-        <v>11.27886336211615</v>
+        <v>1.5289999999999999</v>
       </c>
       <c r="J30">
-        <v>1269.6925560598418</v>
+        <v>970.592783686507</v>
       </c>
       <c r="K30">
-        <v>-7.1605325062720352E-10</v>
+        <v>1.041980747837996E-8</v>
       </c>
       <c r="L30">
         <v>-60</v>
@@ -2423,22 +2423,22 @@
         <v>0</v>
       </c>
       <c r="O30">
-        <v>11.27886336211615</v>
+        <v>1.5289999999999999</v>
       </c>
       <c r="P30">
-        <v>1.8467493551032486</v>
+        <v>2.5480114419962745</v>
       </c>
       <c r="Q30">
-        <v>3.6934987102064971</v>
+        <v>5.096022883992549</v>
       </c>
       <c r="R30">
-        <v>5.5402480653097452</v>
+        <v>7.644034325988823</v>
       </c>
       <c r="S30">
-        <v>1.8467493551032486</v>
+        <v>2.5480114419962745</v>
       </c>
       <c r="T30">
-        <v>10.221399999999999</v>
+        <v>1.3915999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -2461,19 +2461,19 @@
         <v>4.5374000000000008</v>
       </c>
       <c r="G31">
-        <v>98.712689962655134</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H31">
-        <v>19.041903144428762</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I31">
-        <v>1.6220587295826414</v>
+        <v>4.9940000000000007</v>
       </c>
       <c r="J31">
-        <v>970.59278388707787</v>
+        <v>1001.0168016803854</v>
       </c>
       <c r="K31">
-        <v>1.0419807411728632E-8</v>
+        <v>-1.1191716667269941E-9</v>
       </c>
       <c r="L31">
         <v>-60</v>
@@ -2485,22 +2485,22 @@
         <v>0</v>
       </c>
       <c r="O31">
-        <v>1.6220587295826414</v>
+        <v>4.9940000000000007</v>
       </c>
       <c r="P31">
-        <v>2.5480114419962745</v>
+        <v>2.132302591982465</v>
       </c>
       <c r="Q31">
-        <v>5.096022883992549</v>
+        <v>4.2646051839649299</v>
       </c>
       <c r="R31">
-        <v>7.644034325988823</v>
+        <v>6.3969077759473949</v>
       </c>
       <c r="S31">
-        <v>2.5480114419962745</v>
+        <v>2.132302591982465</v>
       </c>
       <c r="T31">
-        <v>1.3915999999999999</v>
+        <v>4.5373999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -2523,19 +2523,19 @@
         <v>1.4210000000000003</v>
       </c>
       <c r="G32">
-        <v>424.16704985282968</v>
+        <v>199.86282285745204</v>
       </c>
       <c r="H32">
-        <v>48.966824396159154</v>
+        <v>40.695483713890681</v>
       </c>
       <c r="I32">
-        <v>5.0103974978387518</v>
+        <v>1.5620000000000001</v>
       </c>
       <c r="J32">
-        <v>1001.2975266341248</v>
+        <v>970.59278377054727</v>
       </c>
       <c r="K32">
-        <v>4.34177318289622E-10</v>
+        <v>1.0419807457454858E-8</v>
       </c>
       <c r="L32">
         <v>-60</v>
@@ -2547,22 +2547,22 @@
         <v>0</v>
       </c>
       <c r="O32">
-        <v>5.0103974978387518</v>
+        <v>1.5620000000000001</v>
       </c>
       <c r="P32">
-        <v>2.132302591982465</v>
+        <v>2.1434788496065242</v>
       </c>
       <c r="Q32">
-        <v>4.2646051839649299</v>
+        <v>4.2869576992130485</v>
       </c>
       <c r="R32">
-        <v>6.3969077759473949</v>
+        <v>6.4304365488195732</v>
       </c>
       <c r="S32">
-        <v>2.132302591982465</v>
+        <v>2.1434788496065242</v>
       </c>
       <c r="T32">
-        <v>4.5373999999999999</v>
+        <v>1.421</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
@@ -2585,19 +2585,19 @@
         <v>3.8906000000000005</v>
       </c>
       <c r="G33">
-        <v>184.8166686745268</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H33">
-        <v>80.336960528575375</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I33">
-        <v>1.5622263602467443</v>
+        <v>4.2790000000000008</v>
       </c>
       <c r="J33">
-        <v>970.5927838120765</v>
+        <v>1186.0087264836197</v>
       </c>
       <c r="K33">
-        <v>1.0419807350335684E-8</v>
+        <v>2.8130698778600204E-10</v>
       </c>
       <c r="L33">
         <v>-60</v>
@@ -2609,22 +2609,22 @@
         <v>0</v>
       </c>
       <c r="O33">
-        <v>1.5622263602467443</v>
+        <v>4.2790000000000008</v>
       </c>
       <c r="P33">
-        <v>2.1434788496065242</v>
+        <v>0.95799035983516656</v>
       </c>
       <c r="Q33">
-        <v>4.2869576992130485</v>
+        <v>1.9159807196703331</v>
       </c>
       <c r="R33">
-        <v>6.4304365488195732</v>
+        <v>2.8739710795054996</v>
       </c>
       <c r="S33">
-        <v>2.1434788496065242</v>
+        <v>0.95799035983516656</v>
       </c>
       <c r="T33">
-        <v>1.421</v>
+        <v>3.8906000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
@@ -2647,19 +2647,19 @@
         <v>8.6044000000000018</v>
       </c>
       <c r="G34">
-        <v>624.0602143042222</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H34">
-        <v>66.651759489751697</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I34">
-        <v>4.2816586464267763</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="J34">
-        <v>1285.516486231061</v>
+        <v>1055.8832574183234</v>
       </c>
       <c r="K34">
-        <v>-6.9103501679860699E-10</v>
+        <v>1.2094970151201853E-9</v>
       </c>
       <c r="L34">
         <v>-60</v>
@@ -2671,22 +2671,22 @@
         <v>0</v>
       </c>
       <c r="O34">
-        <v>4.2816586464267763</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="P34">
-        <v>0.95799035983516656</v>
+        <v>2.3377851878514901</v>
       </c>
       <c r="Q34">
-        <v>1.9159807196703331</v>
+        <v>4.6755703757029803</v>
       </c>
       <c r="R34">
-        <v>2.8739710795054996</v>
+        <v>7.0133555635544704</v>
       </c>
       <c r="S34">
-        <v>0.95799035983516656</v>
+        <v>2.3377851878514901</v>
       </c>
       <c r="T34">
-        <v>3.8906000000000001</v>
+        <v>8.6044</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
@@ -2709,19 +2709,19 @@
         <v>3.5378000000000007</v>
       </c>
       <c r="G35">
-        <v>721.22816043964588</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H35">
-        <v>85.5479769151287</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I35">
-        <v>9.5161090938986561</v>
+        <v>3.8940000000000006</v>
       </c>
       <c r="J35">
-        <v>1056.393015274745</v>
+        <v>979.68498719701654</v>
       </c>
       <c r="K35">
-        <v>1.4301431281906407E-9</v>
+        <v>-4.1503033988069722E-11</v>
       </c>
       <c r="L35">
         <v>-60</v>
@@ -2733,22 +2733,22 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <v>9.5161090938986561</v>
+        <v>3.8940000000000006</v>
       </c>
       <c r="P35">
-        <v>2.3377851878514901</v>
+        <v>2.1183837263904857</v>
       </c>
       <c r="Q35">
-        <v>4.6755703757029803</v>
+        <v>4.2367674527809713</v>
       </c>
       <c r="R35">
-        <v>7.0133555635544704</v>
+        <v>6.3551511791714574</v>
       </c>
       <c r="S35">
-        <v>2.3377851878514901</v>
+        <v>2.1183837263904857</v>
       </c>
       <c r="T35">
-        <v>8.6044</v>
+        <v>3.5377999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
@@ -2771,19 +2771,19 @@
         <v>16.473800000000001</v>
       </c>
       <c r="G36">
-        <v>488.89793809475486</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H36">
-        <v>69.810021125597245</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I36">
-        <v>3.9057180329452308</v>
+        <v>18.117000000000001</v>
       </c>
       <c r="J36">
-        <v>979.94293781214071</v>
+        <v>1791.0895303903144</v>
       </c>
       <c r="K36">
-        <v>-3.6813430471282574E-10</v>
+        <v>1.0442588488315411E-11</v>
       </c>
       <c r="L36">
         <v>-60</v>
@@ -2795,22 +2795,22 @@
         <v>0</v>
       </c>
       <c r="O36">
-        <v>3.9057180329452308</v>
+        <v>18.117000000000001</v>
       </c>
       <c r="P36">
-        <v>2.1183837263904857</v>
+        <v>2.2304969312426666</v>
       </c>
       <c r="Q36">
-        <v>4.2367674527809713</v>
+        <v>4.4609938624853331</v>
       </c>
       <c r="R36">
-        <v>6.3551511791714574</v>
+        <v>6.6914907937279997</v>
       </c>
       <c r="S36">
-        <v>2.1183837263904857</v>
+        <v>2.2304969312426666</v>
       </c>
       <c r="T36">
-        <v>3.5377999999999998</v>
+        <v>16.473800000000001</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
@@ -2833,19 +2833,19 @@
         <v>2.5480000000000005</v>
       </c>
       <c r="G37">
-        <v>458.84899943615301</v>
+        <v>365.81617683817126</v>
       </c>
       <c r="H37">
-        <v>98.305360773035687</v>
+        <v>76.350464084881338</v>
       </c>
       <c r="I37">
-        <v>2.8102156122296753</v>
+        <v>2.8050000000000002</v>
       </c>
       <c r="J37">
-        <v>1050.5051396805911</v>
+        <v>970.59278824211242</v>
       </c>
       <c r="K37">
-        <v>-1.3193100092306163E-9</v>
+        <v>1.0419807493884051E-8</v>
       </c>
       <c r="L37">
         <v>-60</v>
@@ -2857,7 +2857,7 @@
         <v>0</v>
       </c>
       <c r="O37">
-        <v>2.8102156122296753</v>
+        <v>2.8050000000000002</v>
       </c>
       <c r="P37">
         <v>1.8253803547622955</v>
@@ -2895,19 +2895,19 @@
         <v>14.866600000000002</v>
       </c>
       <c r="G38">
-        <v>624.06207006433658</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H38">
-        <v>66.634980020661928</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I38">
-        <v>16.430704765063748</v>
+        <v>16.356999999999999</v>
       </c>
       <c r="J38">
-        <v>1485.7961608793548</v>
+        <v>2750.1933754293727</v>
       </c>
       <c r="K38">
-        <v>3.3350101376978247E-10</v>
+        <v>7.9590768746284685E-11</v>
       </c>
       <c r="L38">
         <v>-60</v>
@@ -2919,7 +2919,7 @@
         <v>0</v>
       </c>
       <c r="O38">
-        <v>16.430704765063748</v>
+        <v>16.356999999999999</v>
       </c>
       <c r="P38">
         <v>2.0673544330144757</v>
@@ -2957,19 +2957,19 @@
         <v>6.0760000000000005</v>
       </c>
       <c r="G39">
-        <v>721.22779842413888</v>
+        <v>479.46322494888784</v>
       </c>
       <c r="H39">
-        <v>85.550597205613826</v>
+        <v>63.93169610401084</v>
       </c>
       <c r="I39">
-        <v>6.6919537142631276</v>
+        <v>6.6880000000000006</v>
       </c>
       <c r="J39">
-        <v>1125.1937992790065</v>
+        <v>1026.043406070567</v>
       </c>
       <c r="K39">
-        <v>7.6972417229576273E-10</v>
+        <v>-7.2066333223714473E-11</v>
       </c>
       <c r="L39">
         <v>-60</v>
@@ -2981,7 +2981,7 @@
         <v>0</v>
       </c>
       <c r="O39">
-        <v>6.6919537142631276</v>
+        <v>6.6880000000000006</v>
       </c>
       <c r="P39">
         <v>2.004574802018523</v>

</xml_diff>

<commit_message>
Iterative Animatlab Testing for Tension Calculation Artifacts
- CanvasModel: stimulus objects now include properties for both simulation equations andproject equations
- parameter_injector: clarified LT parameters and reduced confusing setup fro incorporating Johnson information
</commit_message>
<xml_diff>
--- a/ParameterCalculation/MuscleParameters_20190513.xlsx
+++ b/ParameterCalculation/MuscleParameters_20190513.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Muscle Name</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>MaximumTension</t>
+  </si>
+  <si>
+    <t>LTLowerOutput</t>
+  </si>
+  <si>
+    <t>LTUpperOutput</t>
   </si>
 </sst>
 </file>
@@ -566,9 +572,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T39"/>
+  <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G2" sqref="G2:T39"/>
     </sheetView>
@@ -581,7 +587,7 @@
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,8 +648,14 @@
       <c r="T1" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -663,19 +675,19 @@
         <v>12.210800000000003</v>
       </c>
       <c r="G2">
-        <v>479.46322494888784</v>
+        <v>964.88884599099606</v>
       </c>
       <c r="H2">
-        <v>63.93169610401084</v>
+        <v>74.811260244959058</v>
       </c>
       <c r="I2">
-        <v>13.431000000000003</v>
+        <v>13.145647045527577</v>
       </c>
       <c r="J2">
-        <v>1765.2638143334184</v>
+        <v>1466.758907373717</v>
       </c>
       <c r="K2">
-        <v>-2.0333978062304618E-10</v>
+        <v>-3.037017895234414E-10</v>
       </c>
       <c r="L2">
         <v>-60</v>
@@ -687,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>13.431000000000003</v>
+        <v>13.145647045527577</v>
       </c>
       <c r="P2">
         <v>1.0740679384557621</v>
@@ -704,8 +716,14 @@
       <c r="T2">
         <v>12.210800000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -725,19 +743,19 @@
         <v>1.0388000000000002</v>
       </c>
       <c r="G3">
-        <v>365.81617683817126</v>
+        <v>678.73515527014069</v>
       </c>
       <c r="H3">
-        <v>76.350464084881338</v>
+        <v>81.730322545787118</v>
       </c>
       <c r="I3">
-        <v>1.1440000000000001</v>
+        <v>1.0928349287931978</v>
       </c>
       <c r="J3">
-        <v>970.5927828387305</v>
+        <v>970.59278274444898</v>
       </c>
       <c r="K3">
-        <v>1.0419807356569846E-8</v>
+        <v>1.041980739091195E-8</v>
       </c>
       <c r="L3">
         <v>-60</v>
@@ -749,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1.1440000000000001</v>
+        <v>1.0928349287931978</v>
       </c>
       <c r="P3">
         <v>0.6819514577231951</v>
@@ -766,8 +784,14 @@
       <c r="T3">
         <v>1.0387999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -787,19 +811,19 @@
         <v>3.0184000000000006</v>
       </c>
       <c r="G4">
-        <v>479.46322494888784</v>
+        <v>915.73552806280247</v>
       </c>
       <c r="H4">
-        <v>63.93169610401084</v>
+        <v>99.61347272280122</v>
       </c>
       <c r="I4">
-        <v>3.3220000000000005</v>
+        <v>3.1769195706595172</v>
       </c>
       <c r="J4">
-        <v>970.59279085163746</v>
+        <v>970.59279007495456</v>
       </c>
       <c r="K4">
-        <v>1.0419807461005621E-8</v>
+        <v>1.0419807446802572E-8</v>
       </c>
       <c r="L4">
         <v>-60</v>
@@ -811,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>3.3220000000000005</v>
+        <v>3.1769195706595172</v>
       </c>
       <c r="P4">
         <v>1.4754747575459182</v>
@@ -820,7 +844,7 @@
         <v>2.9509495150918363</v>
       </c>
       <c r="R4">
-        <v>4.426424272637755</v>
+        <v>4.4264242726377541</v>
       </c>
       <c r="S4">
         <v>1.4754747575459182</v>
@@ -828,8 +852,14 @@
       <c r="T4">
         <v>3.0184000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -849,19 +879,19 @@
         <v>3.3908000000000005</v>
       </c>
       <c r="G5">
-        <v>365.81617683817126</v>
+        <v>568.82366725520308</v>
       </c>
       <c r="H5">
-        <v>76.350464084881338</v>
+        <v>50.850852250497354</v>
       </c>
       <c r="I5">
-        <v>3.7290000000000005</v>
+        <v>3.5719368323964606</v>
       </c>
       <c r="J5">
-        <v>1074.905534196183</v>
+        <v>1071.194839902483</v>
       </c>
       <c r="K5">
-        <v>1.4681972756055362E-9</v>
+        <v>-8.7439164888269988E-10</v>
       </c>
       <c r="L5">
         <v>-60</v>
@@ -873,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>3.7290000000000005</v>
+        <v>3.5719368323964606</v>
       </c>
       <c r="P5">
         <v>2.6026604179888015</v>
@@ -890,8 +920,14 @@
       <c r="T5">
         <v>3.3908</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -911,19 +947,19 @@
         <v>12.485200000000003</v>
       </c>
       <c r="G6">
-        <v>479.46322494888784</v>
+        <v>964.88882338151734</v>
       </c>
       <c r="H6">
-        <v>63.93169610401084</v>
+        <v>74.81186942671296</v>
       </c>
       <c r="I6">
-        <v>13.739000000000001</v>
+        <v>13.401717805426239</v>
       </c>
       <c r="J6">
-        <v>1766.8955992803633</v>
+        <v>1468.4398847014936</v>
       </c>
       <c r="K6">
-        <v>-1.3013249591551181E-11</v>
+        <v>-3.7380744457714575E-10</v>
       </c>
       <c r="L6">
         <v>-60</v>
@@ -935,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>13.739000000000001</v>
+        <v>13.401717805426239</v>
       </c>
       <c r="P6">
         <v>2.2577542121616823</v>
@@ -944,7 +980,7 @@
         <v>4.5155084243233645</v>
       </c>
       <c r="R6">
-        <v>6.7732626364850468</v>
+        <v>6.7732626364850477</v>
       </c>
       <c r="S6">
         <v>2.2577542121616823</v>
@@ -952,8 +988,14 @@
       <c r="T6">
         <v>12.485200000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -973,19 +1015,19 @@
         <v>2.0580000000000003</v>
       </c>
       <c r="G7">
-        <v>44.454092278238491</v>
+        <v>421.76128762635472</v>
       </c>
       <c r="H7">
-        <v>75.493326723117917</v>
+        <v>53.834250142366173</v>
       </c>
       <c r="I7">
-        <v>2.2660000000000005</v>
+        <v>2.1683805007596577</v>
       </c>
       <c r="J7">
-        <v>970.59278599053619</v>
+        <v>970.59278563392297</v>
       </c>
       <c r="K7">
-        <v>1.0419807395113233E-8</v>
+        <v>1.0419807399748198E-8</v>
       </c>
       <c r="L7">
         <v>-60</v>
@@ -997,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>2.2660000000000005</v>
+        <v>2.1683805007596577</v>
       </c>
       <c r="P7">
         <v>2.1367296848367752</v>
@@ -1014,8 +1056,14 @@
       <c r="T7">
         <v>2.0579999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1035,19 +1083,19 @@
         <v>2.21</v>
       </c>
       <c r="G8">
-        <v>199.86282285745204</v>
+        <v>278.49823038262019</v>
       </c>
       <c r="H8">
-        <v>40.695483713890681</v>
+        <v>26.297105824708328</v>
       </c>
       <c r="I8">
-        <v>2.431</v>
+        <v>2.335391876121987</v>
       </c>
       <c r="J8">
-        <v>970.59278662901943</v>
+        <v>970.59278625362197</v>
       </c>
       <c r="K8">
-        <v>1.041980746068036E-8</v>
+        <v>1.041980745569303E-8</v>
       </c>
       <c r="L8">
         <v>-60</v>
@@ -1059,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>2.431</v>
+        <v>2.335391876121987</v>
       </c>
       <c r="P8">
         <v>3.3675065648772344</v>
@@ -1068,7 +1116,7 @@
         <v>6.7350131297544689</v>
       </c>
       <c r="R8">
-        <v>10.102519694631702</v>
+        <v>10.102519694631704</v>
       </c>
       <c r="S8">
         <v>3.3675065648772344</v>
@@ -1076,8 +1124,14 @@
       <c r="T8">
         <v>2.21</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1097,19 +1151,19 @@
         <v>11.015200000000002</v>
       </c>
       <c r="G9">
-        <v>479.46322494888784</v>
+        <v>964.88869917520151</v>
       </c>
       <c r="H9">
-        <v>63.93169610401084</v>
+        <v>74.813658551431971</v>
       </c>
       <c r="I9">
-        <v>12.122</v>
+        <v>11.752059621817782</v>
       </c>
       <c r="J9">
-        <v>2712.2260469545163</v>
+        <v>2640.3081292059028</v>
       </c>
       <c r="K9">
-        <v>9.8994955296440991E-11</v>
+        <v>2.7539838294205119E-10</v>
       </c>
       <c r="L9">
         <v>-60</v>
@@ -1121,7 +1175,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>12.122</v>
+        <v>11.752059621817782</v>
       </c>
       <c r="P9">
         <v>3.1770497211103974</v>
@@ -1138,8 +1192,14 @@
       <c r="T9">
         <v>11.0152</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1159,19 +1219,19 @@
         <v>0.44100000000000006</v>
       </c>
       <c r="G10">
-        <v>21.555887203496994</v>
+        <v>11.680991130339603</v>
       </c>
       <c r="H10">
-        <v>55.984070587250969</v>
+        <v>53.990509384962529</v>
       </c>
       <c r="I10">
-        <v>0.48400000000000004</v>
+        <v>0.48510000000000003</v>
       </c>
       <c r="J10">
-        <v>970.59278195359286</v>
+        <v>970.59278195447371</v>
       </c>
       <c r="K10">
-        <v>1.0419807394977708E-8</v>
+        <v>1.0419807408204975E-8</v>
       </c>
       <c r="L10">
         <v>-60</v>
@@ -1183,7 +1243,7 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>0.48400000000000004</v>
+        <v>0.48510000000000003</v>
       </c>
       <c r="P10">
         <v>3.071691927986151</v>
@@ -1192,7 +1252,7 @@
         <v>6.143383855972302</v>
       </c>
       <c r="R10">
-        <v>9.2150757839584525</v>
+        <v>9.2150757839584543</v>
       </c>
       <c r="S10">
         <v>3.071691927986151</v>
@@ -1200,8 +1260,14 @@
       <c r="T10">
         <v>0.441</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1221,19 +1287,19 @@
         <v>2.8518000000000003</v>
       </c>
       <c r="G11">
-        <v>479.46322494888784</v>
+        <v>964.88854771612228</v>
       </c>
       <c r="H11">
-        <v>63.93169610401084</v>
+        <v>74.815033288348843</v>
       </c>
       <c r="I11">
-        <v>3.1350000000000002</v>
+        <v>3.0495441317618215</v>
       </c>
       <c r="J11">
-        <v>1059.9398293869169</v>
+        <v>970.59278942152343</v>
       </c>
       <c r="K11">
-        <v>1.0122742547722417E-9</v>
+        <v>1.0419807403732641E-8</v>
       </c>
       <c r="L11">
         <v>-60</v>
@@ -1245,7 +1311,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>3.1350000000000002</v>
+        <v>3.0495441317618215</v>
       </c>
       <c r="P11">
         <v>0.7143478013034501</v>
@@ -1254,7 +1320,7 @@
         <v>1.4286956026069002</v>
       </c>
       <c r="R11">
-        <v>2.1430434039103501</v>
+        <v>2.1430434039103505</v>
       </c>
       <c r="S11">
         <v>0.7143478013034501</v>
@@ -1262,8 +1328,14 @@
       <c r="T11">
         <v>2.8517999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1283,19 +1355,19 @@
         <v>0.37240000000000006</v>
       </c>
       <c r="G12">
-        <v>44.454092278238491</v>
+        <v>473.28884901734483</v>
       </c>
       <c r="H12">
-        <v>75.493326723117917</v>
+        <v>45.092370491063313</v>
       </c>
       <c r="I12">
-        <v>0.40700000000000003</v>
+        <v>0.39249357227766013</v>
       </c>
       <c r="J12">
-        <v>970.59278189707743</v>
+        <v>970.59278188752467</v>
       </c>
       <c r="K12">
-        <v>1.0419807379283882E-8</v>
+        <v>1.0419807397037692E-8</v>
       </c>
       <c r="L12">
         <v>-60</v>
@@ -1307,7 +1379,7 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>0.40700000000000003</v>
+        <v>0.39249357227766013</v>
       </c>
       <c r="P12">
         <v>0.34469225101316964</v>
@@ -1324,8 +1396,14 @@
       <c r="T12">
         <v>0.37240000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1345,19 +1423,19 @@
         <v>9.231600000000002</v>
       </c>
       <c r="G13">
-        <v>479.46322494888784</v>
+        <v>964.88871191524186</v>
       </c>
       <c r="H13">
-        <v>63.93169610401084</v>
+        <v>74.812950647122634</v>
       </c>
       <c r="I13">
-        <v>10.153</v>
+        <v>9.9370259733224859</v>
       </c>
       <c r="J13">
-        <v>1444.711873773193</v>
+        <v>1159.3170658306813</v>
       </c>
       <c r="K13">
-        <v>-2.1138595844171893E-10</v>
+        <v>6.0470358634197102E-10</v>
       </c>
       <c r="L13">
         <v>-60</v>
@@ -1369,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>10.153</v>
+        <v>9.9370259733224859</v>
       </c>
       <c r="P13">
         <v>0.86496146254423367</v>
@@ -1386,8 +1464,14 @@
       <c r="T13">
         <v>9.2316000000000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1407,19 +1491,19 @@
         <v>18.737600000000004</v>
       </c>
       <c r="G14">
-        <v>479.46322494888784</v>
+        <v>964.88928153288055</v>
       </c>
       <c r="H14">
-        <v>63.93169610401084</v>
+        <v>74.805650097005241</v>
       </c>
       <c r="I14">
-        <v>20.614000000000001</v>
+        <v>20.182549049010248</v>
       </c>
       <c r="J14">
-        <v>1323.6415507499746</v>
+        <v>2682.8508105830679</v>
       </c>
       <c r="K14">
-        <v>-4.9539255537442846E-9</v>
+        <v>3.3092476398125879E-10</v>
       </c>
       <c r="L14">
         <v>-60</v>
@@ -1431,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>20.614000000000001</v>
+        <v>20.182549049010248</v>
       </c>
       <c r="P14">
         <v>1.0969792064708848</v>
@@ -1440,7 +1524,7 @@
         <v>2.1939584129417695</v>
       </c>
       <c r="R14">
-        <v>3.2909376194126541</v>
+        <v>3.2909376194126545</v>
       </c>
       <c r="S14">
         <v>1.0969792064708848</v>
@@ -1448,8 +1532,14 @@
       <c r="T14">
         <v>18.7376</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1469,19 +1559,19 @@
         <v>7.3892000000000007</v>
       </c>
       <c r="G15">
-        <v>479.46322494888784</v>
+        <v>964.88864774092247</v>
       </c>
       <c r="H15">
-        <v>63.93169610401084</v>
+        <v>74.813759046526911</v>
       </c>
       <c r="I15">
-        <v>8.1289999999999996</v>
+        <v>7.9526130544060614</v>
       </c>
       <c r="J15">
-        <v>1042.8159564824132</v>
+        <v>1338.9807124916722</v>
       </c>
       <c r="K15">
-        <v>1.1185604763214426E-9</v>
+        <v>-2.2486144722030136E-10</v>
       </c>
       <c r="L15">
         <v>-60</v>
@@ -1493,7 +1583,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>8.1289999999999996</v>
+        <v>7.9526130544060614</v>
       </c>
       <c r="P15">
         <v>0.73964612772368377</v>
@@ -1510,8 +1600,14 @@
       <c r="T15">
         <v>7.3891999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1531,19 +1627,19 @@
         <v>1.5484000000000002</v>
       </c>
       <c r="G16">
-        <v>44.454092278238491</v>
+        <v>421.76129159610463</v>
       </c>
       <c r="H16">
-        <v>75.493326723117917</v>
+        <v>53.834247451610452</v>
       </c>
       <c r="I16">
-        <v>1.7050000000000003</v>
+        <v>1.6439173193557928</v>
       </c>
       <c r="J16">
-        <v>970.59278415537017</v>
+        <v>970.59278398685319</v>
       </c>
       <c r="K16">
-        <v>1.0419807411349161E-8</v>
+        <v>1.041980744330602E-8</v>
       </c>
       <c r="L16">
         <v>-60</v>
@@ -1555,7 +1651,7 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>1.7050000000000003</v>
+        <v>1.6439173193557928</v>
       </c>
       <c r="P16">
         <v>1.5229111097674977</v>
@@ -1572,8 +1668,14 @@
       <c r="T16">
         <v>1.5484</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1593,19 +1695,19 @@
         <v>2.3520000000000003</v>
       </c>
       <c r="G17">
-        <v>365.81617683817126</v>
+        <v>616.04467794214827</v>
       </c>
       <c r="H17">
-        <v>76.350464084881338</v>
+        <v>64.774596643737524</v>
       </c>
       <c r="I17">
-        <v>2.5850000000000004</v>
+        <v>2.4738509630360879</v>
       </c>
       <c r="J17">
-        <v>970.59278726535365</v>
+        <v>970.59278680211412</v>
       </c>
       <c r="K17">
-        <v>1.041980744083946E-8</v>
+        <v>1.0419807296938727E-8</v>
       </c>
       <c r="L17">
         <v>-60</v>
@@ -1617,7 +1719,7 @@
         <v>0</v>
       </c>
       <c r="O17">
-        <v>2.5850000000000004</v>
+        <v>2.4738509630360879</v>
       </c>
       <c r="P17">
         <v>1.7213459986255004</v>
@@ -1626,7 +1728,7 @@
         <v>3.4426919972510008</v>
       </c>
       <c r="R17">
-        <v>5.1640379958765017</v>
+        <v>5.1640379958765008</v>
       </c>
       <c r="S17">
         <v>1.7213459986255004</v>
@@ -1634,8 +1736,14 @@
       <c r="T17">
         <v>2.3519999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1655,19 +1763,19 @@
         <v>11.279800000000002</v>
       </c>
       <c r="G18">
-        <v>479.46322494888784</v>
+        <v>964.88880518137353</v>
       </c>
       <c r="H18">
-        <v>63.93169610401084</v>
+        <v>74.811722856105362</v>
       </c>
       <c r="I18">
-        <v>12.407999999999999</v>
+        <v>12.14907527107299</v>
       </c>
       <c r="J18">
-        <v>1876.3450388558454</v>
+        <v>2708.7983118464754</v>
       </c>
       <c r="K18">
-        <v>-1.8048018280388312E-10</v>
+        <v>1.541267112547455E-10</v>
       </c>
       <c r="L18">
         <v>-60</v>
@@ -1679,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>12.407999999999999</v>
+        <v>12.14907527107299</v>
       </c>
       <c r="P18">
         <v>0.68705617240035788</v>
@@ -1688,7 +1796,7 @@
         <v>1.3741123448007158</v>
       </c>
       <c r="R18">
-        <v>2.0611685172010734</v>
+        <v>2.0611685172010739</v>
       </c>
       <c r="S18">
         <v>0.68705617240035788</v>
@@ -1696,8 +1804,14 @@
       <c r="T18">
         <v>11.2798</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1717,19 +1831,19 @@
         <v>18.257400000000004</v>
       </c>
       <c r="G19">
-        <v>479.46322494888784</v>
+        <v>964.88918997934377</v>
       </c>
       <c r="H19">
-        <v>63.93169610401084</v>
+        <v>74.807348314114719</v>
       </c>
       <c r="I19">
-        <v>20.086000000000002</v>
+        <v>19.625673516085332</v>
       </c>
       <c r="J19">
-        <v>1799.818113478547</v>
+        <v>2661.902697733894</v>
       </c>
       <c r="K19">
-        <v>-1.7398939151253088E-10</v>
+        <v>3.8358256458846791E-10</v>
       </c>
       <c r="L19">
         <v>-60</v>
@@ -1741,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <v>20.086000000000002</v>
+        <v>19.625673516085332</v>
       </c>
       <c r="P19">
         <v>2.6669440174759429</v>
@@ -1758,8 +1872,14 @@
       <c r="T19">
         <v>18.257400000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1779,19 +1899,19 @@
         <v>11.642400000000002</v>
       </c>
       <c r="G20">
-        <v>479.46322494888784</v>
+        <v>964.88876651303963</v>
       </c>
       <c r="H20">
-        <v>63.93169610401084</v>
+        <v>74.812670861443991</v>
       </c>
       <c r="I20">
-        <v>12.804000000000002</v>
+        <v>12.475160347433974</v>
       </c>
       <c r="J20">
-        <v>1661.7803694415495</v>
+        <v>2674.8754161982774</v>
       </c>
       <c r="K20">
-        <v>3.0012552151959176E-10</v>
+        <v>2.2002590050442099E-10</v>
       </c>
       <c r="L20">
         <v>-60</v>
@@ -1803,7 +1923,7 @@
         <v>0</v>
       </c>
       <c r="O20">
-        <v>12.804000000000002</v>
+        <v>12.475160347433974</v>
       </c>
       <c r="P20">
         <v>2.5324667381562982</v>
@@ -1812,7 +1932,7 @@
         <v>5.0649334763125964</v>
       </c>
       <c r="R20">
-        <v>7.5974002144688946</v>
+        <v>7.5974002144688937</v>
       </c>
       <c r="S20">
         <v>2.5324667381562982</v>
@@ -1820,8 +1940,14 @@
       <c r="T20">
         <v>11.6424</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1841,19 +1967,19 @@
         <v>7.1736000000000013</v>
       </c>
       <c r="G21">
-        <v>479.46322494888784</v>
+        <v>964.88864326542819</v>
       </c>
       <c r="H21">
-        <v>63.93169610401084</v>
+        <v>74.813794837360874</v>
       </c>
       <c r="I21">
-        <v>7.8870000000000005</v>
+        <v>7.7243138631023456</v>
       </c>
       <c r="J21">
-        <v>1338.2590390464227</v>
+        <v>1137.5558097438584</v>
       </c>
       <c r="K21">
-        <v>-1.0980806543315517E-9</v>
+        <v>6.5796688754694911E-10</v>
       </c>
       <c r="L21">
         <v>-60</v>
@@ -1865,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="O21">
-        <v>7.8870000000000005</v>
+        <v>7.7243138631023456</v>
       </c>
       <c r="P21">
         <v>0.55396022614012119</v>
@@ -1874,7 +2000,7 @@
         <v>1.1079204522802424</v>
       </c>
       <c r="R21">
-        <v>1.6618806784203635</v>
+        <v>1.6618806784203637</v>
       </c>
       <c r="S21">
         <v>0.55396022614012119</v>
@@ -1882,8 +2008,14 @@
       <c r="T21">
         <v>7.1736000000000004</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1903,19 +2035,19 @@
         <v>3.0086000000000004</v>
       </c>
       <c r="G22">
-        <v>479.46322494888784</v>
+        <v>964.88854966560007</v>
       </c>
       <c r="H22">
-        <v>63.93169610401084</v>
+        <v>74.815009864657128</v>
       </c>
       <c r="I22">
-        <v>3.3109999999999999</v>
+        <v>3.2195416042945957</v>
       </c>
       <c r="J22">
-        <v>970.5927907915642</v>
+        <v>1062.2355830163558</v>
       </c>
       <c r="K22">
-        <v>1.0419807369227907E-8</v>
+        <v>-2.2053187999478748E-10</v>
       </c>
       <c r="L22">
         <v>-60</v>
@@ -1927,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="O22">
-        <v>3.3109999999999999</v>
+        <v>3.2195416042945957</v>
       </c>
       <c r="P22">
         <v>0.71754839180542296</v>
@@ -1944,8 +2076,14 @@
       <c r="T22">
         <v>3.0085999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1965,19 +2103,19 @@
         <v>4.9294000000000011</v>
       </c>
       <c r="G23">
-        <v>479.46322494888784</v>
+        <v>964.88857654747244</v>
       </c>
       <c r="H23">
-        <v>63.93169610401084</v>
+        <v>74.814713295142425</v>
       </c>
       <c r="I23">
-        <v>5.423</v>
+        <v>5.2817037656136305</v>
       </c>
       <c r="J23">
-        <v>1305.9138355421981</v>
+        <v>1104.849921619199</v>
       </c>
       <c r="K23">
-        <v>-3.0927586036675757E-10</v>
+        <v>-8.4179267142585563E-10</v>
       </c>
       <c r="L23">
         <v>-60</v>
@@ -1989,7 +2127,7 @@
         <v>0</v>
       </c>
       <c r="O23">
-        <v>5.423</v>
+        <v>5.2817037656136305</v>
       </c>
       <c r="P23">
         <v>1.0651425852178873</v>
@@ -2006,8 +2144,14 @@
       <c r="T23">
         <v>4.9294000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2027,19 +2171,19 @@
         <v>3.9592000000000005</v>
       </c>
       <c r="G24">
-        <v>365.81617683817126</v>
+        <v>655.09800811180151</v>
       </c>
       <c r="H24">
-        <v>76.350464084881338</v>
+        <v>90.271618882562706</v>
       </c>
       <c r="I24">
-        <v>4.3559999999999999</v>
+        <v>4.1617206425261237</v>
       </c>
       <c r="J24">
-        <v>989.30497722942198</v>
+        <v>985.3916138384642</v>
       </c>
       <c r="K24">
-        <v>-5.7586706766882303E-11</v>
+        <v>2.818643873990286E-10</v>
       </c>
       <c r="L24">
         <v>-60</v>
@@ -2051,7 +2195,7 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <v>4.3559999999999999</v>
+        <v>4.1617206425261237</v>
       </c>
       <c r="P24">
         <v>2.6500679504403895</v>
@@ -2060,7 +2204,7 @@
         <v>5.3001359008807789</v>
       </c>
       <c r="R24">
-        <v>7.9502038513211684</v>
+        <v>7.9502038513211692</v>
       </c>
       <c r="S24">
         <v>2.6500679504403895</v>
@@ -2068,8 +2212,14 @@
       <c r="T24">
         <v>3.9592000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2089,19 +2239,19 @@
         <v>11.142600000000002</v>
       </c>
       <c r="G25">
-        <v>479.46322494888784</v>
+        <v>964.88879673119368</v>
       </c>
       <c r="H25">
-        <v>63.93169610401084</v>
+        <v>74.811849965609525</v>
       </c>
       <c r="I25">
-        <v>12.254000000000001</v>
+        <v>11.998977174955817</v>
       </c>
       <c r="J25">
-        <v>1363.0300503908536</v>
+        <v>1854.9271610363492</v>
       </c>
       <c r="K25">
-        <v>2.8670327384551484E-10</v>
+        <v>-1.0768591502512206E-10</v>
       </c>
       <c r="L25">
         <v>-60</v>
@@ -2113,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>12.254000000000001</v>
+        <v>11.998977174955817</v>
       </c>
       <c r="P25">
         <v>0.81547251145974264</v>
@@ -2122,7 +2272,7 @@
         <v>1.6309450229194853</v>
       </c>
       <c r="R25">
-        <v>2.4464175343792278</v>
+        <v>2.4464175343792283</v>
       </c>
       <c r="S25">
         <v>0.81547251145974264</v>
@@ -2130,8 +2280,14 @@
       <c r="T25">
         <v>11.1426</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -2151,19 +2307,19 @@
         <v>5.6056000000000008</v>
       </c>
       <c r="G26">
-        <v>479.46322494888784</v>
+        <v>933.99325128669739</v>
       </c>
       <c r="H26">
-        <v>63.93169610401084</v>
+        <v>77.491036743316656</v>
       </c>
       <c r="I26">
-        <v>6.1710000000000012</v>
+        <v>5.8927578284774143</v>
       </c>
       <c r="J26">
-        <v>1019.1434104915377</v>
+        <v>1114.2568793473195</v>
       </c>
       <c r="K26">
-        <v>2.7320588799080375E-12</v>
+        <v>2.3590254956933913E-10</v>
       </c>
       <c r="L26">
         <v>-60</v>
@@ -2175,7 +2331,7 @@
         <v>0</v>
       </c>
       <c r="O26">
-        <v>6.1710000000000012</v>
+        <v>5.8927578284774143</v>
       </c>
       <c r="P26">
         <v>2.6504213747458651</v>
@@ -2184,7 +2340,7 @@
         <v>5.3008427494917303</v>
       </c>
       <c r="R26">
-        <v>7.9512641242375954</v>
+        <v>7.9512641242375945</v>
       </c>
       <c r="S26">
         <v>2.6504213747458651</v>
@@ -2192,8 +2348,14 @@
       <c r="T26">
         <v>5.6055999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2213,19 +2375,19 @@
         <v>2.9204000000000003</v>
       </c>
       <c r="G27">
-        <v>479.46322494888784</v>
+        <v>964.88854073927814</v>
       </c>
       <c r="H27">
-        <v>63.93169610401084</v>
+        <v>74.815124457131731</v>
       </c>
       <c r="I27">
-        <v>3.2120000000000002</v>
+        <v>3.0897500224106174</v>
       </c>
       <c r="J27">
-        <v>970.59279025946125</v>
+        <v>1157.8746189869605</v>
       </c>
       <c r="K27">
-        <v>1.0419807318378825E-8</v>
+        <v>6.1014888042877422E-10</v>
       </c>
       <c r="L27">
         <v>-60</v>
@@ -2237,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>3.2120000000000002</v>
+        <v>3.0897500224106174</v>
       </c>
       <c r="P27">
         <v>1.1237106940141237</v>
@@ -2246,7 +2408,7 @@
         <v>2.2474213880282474</v>
       </c>
       <c r="R27">
-        <v>3.3711320820423714</v>
+        <v>3.3711320820423709</v>
       </c>
       <c r="S27">
         <v>1.1237106940141237</v>
@@ -2254,8 +2416,14 @@
       <c r="T27">
         <v>2.9203999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2275,19 +2443,19 @@
         <v>2.9988000000000006</v>
       </c>
       <c r="G28">
-        <v>479.46322494888784</v>
+        <v>964.88854828391754</v>
       </c>
       <c r="H28">
-        <v>63.93169610401084</v>
+        <v>74.815032440735692</v>
       </c>
       <c r="I28">
-        <v>3.3000000000000003</v>
+        <v>3.2034547828413027</v>
       </c>
       <c r="J28">
-        <v>970.59279073154835</v>
+        <v>1061.8027426756994</v>
       </c>
       <c r="K28">
-        <v>1.0419807462387978E-8</v>
+        <v>-3.7867167117372203E-10</v>
       </c>
       <c r="L28">
         <v>-60</v>
@@ -2299,7 +2467,7 @@
         <v>0</v>
       </c>
       <c r="O28">
-        <v>3.3000000000000003</v>
+        <v>3.2034547828413027</v>
       </c>
       <c r="P28">
         <v>0.79941043356034458</v>
@@ -2316,8 +2484,14 @@
       <c r="T28">
         <v>2.9988000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -2337,19 +2511,19 @@
         <v>10.221400000000001</v>
       </c>
       <c r="G29">
-        <v>479.46322494888784</v>
+        <v>964.88872804299615</v>
       </c>
       <c r="H29">
-        <v>63.93169610401084</v>
+        <v>74.812957287252473</v>
       </c>
       <c r="I29">
-        <v>11.242000000000001</v>
+        <v>10.9713589889361</v>
       </c>
       <c r="J29">
-        <v>1355.7248731180293</v>
+        <v>2671.6142466358824</v>
       </c>
       <c r="K29">
-        <v>-9.7866131654512724E-11</v>
+        <v>1.9939571669765544E-10</v>
       </c>
       <c r="L29">
         <v>-60</v>
@@ -2361,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="O29">
-        <v>11.242000000000001</v>
+        <v>10.9713589889361</v>
       </c>
       <c r="P29">
         <v>1.8467493551032486</v>
@@ -2378,8 +2552,14 @@
       <c r="T29">
         <v>10.221399999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -2399,19 +2579,19 @@
         <v>1.3916000000000002</v>
       </c>
       <c r="G30">
-        <v>111.70574419320344</v>
+        <v>186.87270608261613</v>
       </c>
       <c r="H30">
-        <v>13.629254893829867</v>
+        <v>40.180914115173088</v>
       </c>
       <c r="I30">
-        <v>1.5289999999999999</v>
+        <v>1.5184932295871971</v>
       </c>
       <c r="J30">
-        <v>970.592783686507</v>
+        <v>970.59278366012438</v>
       </c>
       <c r="K30">
-        <v>1.041980747837996E-8</v>
+        <v>1.0419807446721257E-8</v>
       </c>
       <c r="L30">
         <v>-60</v>
@@ -2423,7 +2603,7 @@
         <v>0</v>
       </c>
       <c r="O30">
-        <v>1.5289999999999999</v>
+        <v>1.5184932295871971</v>
       </c>
       <c r="P30">
         <v>2.5480114419962745</v>
@@ -2432,7 +2612,7 @@
         <v>5.096022883992549</v>
       </c>
       <c r="R30">
-        <v>7.644034325988823</v>
+        <v>7.6440343259888248</v>
       </c>
       <c r="S30">
         <v>2.5480114419962745</v>
@@ -2440,8 +2620,14 @@
       <c r="T30">
         <v>1.3915999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -2461,19 +2647,19 @@
         <v>4.5374000000000008</v>
       </c>
       <c r="G31">
-        <v>479.46322494888784</v>
+        <v>933.99325069382519</v>
       </c>
       <c r="H31">
-        <v>63.93169610401084</v>
+        <v>77.491038054147367</v>
       </c>
       <c r="I31">
-        <v>4.9940000000000007</v>
+        <v>4.7713448069355655</v>
       </c>
       <c r="J31">
-        <v>1001.0168016803854</v>
+        <v>1096.1182949203883</v>
       </c>
       <c r="K31">
-        <v>-1.1191716667269941E-9</v>
+        <v>-1.2506808819957451E-9</v>
       </c>
       <c r="L31">
         <v>-60</v>
@@ -2485,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="O31">
-        <v>4.9940000000000007</v>
+        <v>4.7713448069355655</v>
       </c>
       <c r="P31">
         <v>2.132302591982465</v>
@@ -2494,7 +2680,7 @@
         <v>4.2646051839649299</v>
       </c>
       <c r="R31">
-        <v>6.3969077759473949</v>
+        <v>6.396907775947394</v>
       </c>
       <c r="S31">
         <v>2.132302591982465</v>
@@ -2502,8 +2688,14 @@
       <c r="T31">
         <v>4.5373999999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -2523,19 +2715,19 @@
         <v>1.4210000000000003</v>
       </c>
       <c r="G32">
-        <v>199.86282285745204</v>
+        <v>278.49822404676121</v>
       </c>
       <c r="H32">
-        <v>40.695483713890681</v>
+        <v>26.297117404078548</v>
       </c>
       <c r="I32">
-        <v>1.5620000000000001</v>
+        <v>1.5024828868806321</v>
       </c>
       <c r="J32">
-        <v>970.59278377054727</v>
+        <v>970.59278362027896</v>
       </c>
       <c r="K32">
-        <v>1.0419807457454858E-8</v>
+        <v>1.0419807474070257E-8</v>
       </c>
       <c r="L32">
         <v>-60</v>
@@ -2547,7 +2739,7 @@
         <v>0</v>
       </c>
       <c r="O32">
-        <v>1.5620000000000001</v>
+        <v>1.5024828868806321</v>
       </c>
       <c r="P32">
         <v>2.1434788496065242</v>
@@ -2556,7 +2748,7 @@
         <v>4.2869576992130485</v>
       </c>
       <c r="R32">
-        <v>6.4304365488195732</v>
+        <v>6.4304365488195723</v>
       </c>
       <c r="S32">
         <v>2.1434788496065242</v>
@@ -2564,8 +2756,14 @@
       <c r="T32">
         <v>1.421</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -2585,19 +2783,19 @@
         <v>3.8906000000000005</v>
       </c>
       <c r="G33">
-        <v>479.46322494888784</v>
+        <v>964.88855883211966</v>
       </c>
       <c r="H33">
-        <v>63.93169610401084</v>
+        <v>74.814919157394371</v>
       </c>
       <c r="I33">
-        <v>4.2790000000000008</v>
+        <v>4.1615018566052209</v>
       </c>
       <c r="J33">
-        <v>1186.0087264836197</v>
+        <v>985.38737635073653</v>
       </c>
       <c r="K33">
-        <v>2.8130698778600204E-10</v>
+        <v>1.0583121146627351E-9</v>
       </c>
       <c r="L33">
         <v>-60</v>
@@ -2609,7 +2807,7 @@
         <v>0</v>
       </c>
       <c r="O33">
-        <v>4.2790000000000008</v>
+        <v>4.1615018566052209</v>
       </c>
       <c r="P33">
         <v>0.95799035983516656</v>
@@ -2626,8 +2824,14 @@
       <c r="T33">
         <v>3.8906000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -2647,19 +2851,19 @@
         <v>8.6044000000000018</v>
       </c>
       <c r="G34">
-        <v>479.46322494888784</v>
+        <v>964.88864161078618</v>
       </c>
       <c r="H34">
-        <v>63.93169610401084</v>
+        <v>74.814140874736992</v>
       </c>
       <c r="I34">
-        <v>9.4600000000000009</v>
+        <v>9.1895925250503279</v>
       </c>
       <c r="J34">
-        <v>1055.8832574183234</v>
+        <v>1053.3825394026182</v>
       </c>
       <c r="K34">
-        <v>1.2094970151201853E-9</v>
+        <v>-1.1940753485748233E-9</v>
       </c>
       <c r="L34">
         <v>-60</v>
@@ -2671,7 +2875,7 @@
         <v>0</v>
       </c>
       <c r="O34">
-        <v>9.4600000000000009</v>
+        <v>9.1895925250503279</v>
       </c>
       <c r="P34">
         <v>2.3377851878514901</v>
@@ -2688,8 +2892,14 @@
       <c r="T34">
         <v>8.6044</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -2709,19 +2919,19 @@
         <v>3.5378000000000007</v>
       </c>
       <c r="G35">
-        <v>479.46322494888784</v>
+        <v>757.74013130810215</v>
       </c>
       <c r="H35">
-        <v>63.93169610401084</v>
+        <v>86.869471326886611</v>
       </c>
       <c r="I35">
-        <v>3.8940000000000006</v>
+        <v>3.7159699893297105</v>
       </c>
       <c r="J35">
-        <v>979.68498719701654</v>
+        <v>975.6655932115691</v>
       </c>
       <c r="K35">
-        <v>-4.1503033988069722E-11</v>
+        <v>-1.4793736184780094E-9</v>
       </c>
       <c r="L35">
         <v>-60</v>
@@ -2733,7 +2943,7 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <v>3.8940000000000006</v>
+        <v>3.7159699893297105</v>
       </c>
       <c r="P35">
         <v>2.1183837263904857</v>
@@ -2750,8 +2960,14 @@
       <c r="T35">
         <v>3.5377999999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -2771,19 +2987,19 @@
         <v>16.473800000000001</v>
       </c>
       <c r="G36">
-        <v>479.46322494888784</v>
+        <v>964.88907506157523</v>
       </c>
       <c r="H36">
-        <v>63.93169610401084</v>
+        <v>74.808645733412064</v>
       </c>
       <c r="I36">
-        <v>18.117000000000001</v>
+        <v>17.713936020296618</v>
       </c>
       <c r="J36">
-        <v>1791.0895303903144</v>
+        <v>1788.9655560614408</v>
       </c>
       <c r="K36">
-        <v>1.0442588488315411E-11</v>
+        <v>4.248448781725237E-10</v>
       </c>
       <c r="L36">
         <v>-60</v>
@@ -2795,7 +3011,7 @@
         <v>0</v>
       </c>
       <c r="O36">
-        <v>18.117000000000001</v>
+        <v>17.713936020296618</v>
       </c>
       <c r="P36">
         <v>2.2304969312426666</v>
@@ -2812,8 +3028,14 @@
       <c r="T36">
         <v>16.473800000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -2833,19 +3055,19 @@
         <v>2.5480000000000005</v>
       </c>
       <c r="G37">
-        <v>365.81617683817126</v>
+        <v>616.04468098287487</v>
       </c>
       <c r="H37">
-        <v>76.350464084881338</v>
+        <v>64.774595331191193</v>
       </c>
       <c r="I37">
-        <v>2.8050000000000002</v>
+        <v>2.6860142775201732</v>
       </c>
       <c r="J37">
-        <v>970.59278824211242</v>
+        <v>1046.6094381136468</v>
       </c>
       <c r="K37">
-        <v>1.0419807493884051E-8</v>
+        <v>-1.4407995813703616E-9</v>
       </c>
       <c r="L37">
         <v>-60</v>
@@ -2857,7 +3079,7 @@
         <v>0</v>
       </c>
       <c r="O37">
-        <v>2.8050000000000002</v>
+        <v>2.6860142775201732</v>
       </c>
       <c r="P37">
         <v>1.8253803547622955</v>
@@ -2866,7 +3088,7 @@
         <v>3.6507607095245911</v>
       </c>
       <c r="R37">
-        <v>5.4761410642868871</v>
+        <v>5.4761410642868862</v>
       </c>
       <c r="S37">
         <v>1.8253803547622955</v>
@@ -2874,8 +3096,14 @@
       <c r="T37">
         <v>2.548</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -2895,19 +3123,19 @@
         <v>14.866600000000002</v>
       </c>
       <c r="G38">
-        <v>479.46322494888784</v>
+        <v>964.88897238369441</v>
       </c>
       <c r="H38">
-        <v>63.93169610401084</v>
+        <v>74.809904455026327</v>
       </c>
       <c r="I38">
-        <v>16.356999999999999</v>
+        <v>15.983534723532214</v>
       </c>
       <c r="J38">
-        <v>2750.1933754293727</v>
+        <v>1698.7641484280259</v>
       </c>
       <c r="K38">
-        <v>7.9590768746284685E-11</v>
+        <v>9.638344709179573E-10</v>
       </c>
       <c r="L38">
         <v>-60</v>
@@ -2919,7 +3147,7 @@
         <v>0</v>
       </c>
       <c r="O38">
-        <v>16.356999999999999</v>
+        <v>15.983534723532214</v>
       </c>
       <c r="P38">
         <v>2.0673544330144757</v>
@@ -2936,8 +3164,14 @@
       <c r="T38">
         <v>14.8666</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -2957,19 +3191,19 @@
         <v>6.0760000000000005</v>
       </c>
       <c r="G39">
-        <v>479.46322494888784</v>
+        <v>964.88857479012165</v>
       </c>
       <c r="H39">
-        <v>63.93169610401084</v>
+        <v>74.814842029811473</v>
       </c>
       <c r="I39">
-        <v>6.6880000000000006</v>
+        <v>6.4607326144868784</v>
       </c>
       <c r="J39">
-        <v>1026.043406070567</v>
+        <v>1122.1671551514592</v>
       </c>
       <c r="K39">
-        <v>-7.2066333223714473E-11</v>
+        <v>5.9724377668417267E-10</v>
       </c>
       <c r="L39">
         <v>-60</v>
@@ -2981,7 +3215,7 @@
         <v>0</v>
       </c>
       <c r="O39">
-        <v>6.6880000000000006</v>
+        <v>6.4607326144868784</v>
       </c>
       <c r="P39">
         <v>2.004574802018523</v>
@@ -2997,6 +3231,12 @@
       </c>
       <c r="T39">
         <v>6.0759999999999996</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimizing Animatlab for Limb Position
- Includes routines for Living Machines 2020 Paper
</commit_message>
<xml_diff>
--- a/ParameterCalculation/MuscleParameters_20190513.xlsx
+++ b/ParameterCalculation/MuscleParameters_20190513.xlsx
@@ -675,19 +675,19 @@
         <v>12.210800000000003</v>
       </c>
       <c r="G2">
-        <v>964.88884599099606</v>
+        <v>964.88884562729652</v>
       </c>
       <c r="H2">
-        <v>74.811260244959058</v>
+        <v>74.811264805230593</v>
       </c>
       <c r="I2">
-        <v>13.145647045527577</v>
+        <v>13.145267620013534</v>
       </c>
       <c r="J2">
-        <v>1466.758907373717</v>
+        <v>1681.8927482316692</v>
       </c>
       <c r="K2">
-        <v>-3.037017895234414E-10</v>
+        <v>-3.8316688590874983E-10</v>
       </c>
       <c r="L2">
         <v>-60</v>
@@ -699,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>13.145647045527577</v>
+        <v>13.145267620013534</v>
       </c>
       <c r="P2">
         <v>1.0740679384557621</v>
@@ -743,19 +743,19 @@
         <v>1.0388000000000002</v>
       </c>
       <c r="G3">
-        <v>678.73515527014069</v>
+        <v>678.73515526746507</v>
       </c>
       <c r="H3">
-        <v>81.730322545787118</v>
+        <v>81.730322542628571</v>
       </c>
       <c r="I3">
-        <v>1.0928349287931978</v>
+        <v>1.0928213395648341</v>
       </c>
       <c r="J3">
-        <v>970.59278274444898</v>
+        <v>970.59278274442465</v>
       </c>
       <c r="K3">
-        <v>1.041980739091195E-8</v>
+        <v>1.0419807390234324E-8</v>
       </c>
       <c r="L3">
         <v>-60</v>
@@ -767,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1.0928349287931978</v>
+        <v>1.0928213395648341</v>
       </c>
       <c r="P3">
         <v>0.6819514577231951</v>
@@ -811,19 +811,19 @@
         <v>3.0184000000000006</v>
       </c>
       <c r="G4">
-        <v>915.73552806280247</v>
+        <v>915.7355279937052</v>
       </c>
       <c r="H4">
-        <v>99.61347272280122</v>
+        <v>99.61347269596277</v>
       </c>
       <c r="I4">
-        <v>3.1769195706595172</v>
+        <v>3.1767368924536519</v>
       </c>
       <c r="J4">
-        <v>970.59279007495456</v>
+        <v>970.59279007387033</v>
       </c>
       <c r="K4">
-        <v>1.0419807446802572E-8</v>
+        <v>1.0419807505105544E-8</v>
       </c>
       <c r="L4">
         <v>-60</v>
@@ -835,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>3.1769195706595172</v>
+        <v>3.1767368924536519</v>
       </c>
       <c r="P4">
         <v>1.4754747575459182</v>
@@ -879,19 +879,19 @@
         <v>3.3908000000000005</v>
       </c>
       <c r="G5">
-        <v>568.82366725520308</v>
+        <v>568.82366691035327</v>
       </c>
       <c r="H5">
-        <v>50.850852250497354</v>
+        <v>50.850852959614393</v>
       </c>
       <c r="I5">
-        <v>3.5719368323964606</v>
+        <v>3.5713104474987101</v>
       </c>
       <c r="J5">
-        <v>1071.194839902483</v>
+        <v>972.254092343146</v>
       </c>
       <c r="K5">
-        <v>-8.7439164888269988E-10</v>
+        <v>-5.9805267946958673E-10</v>
       </c>
       <c r="L5">
         <v>-60</v>
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>3.5719368323964606</v>
+        <v>3.5713104474987101</v>
       </c>
       <c r="P5">
         <v>2.6026604179888015</v>
@@ -947,19 +947,19 @@
         <v>12.485200000000003</v>
       </c>
       <c r="G6">
-        <v>964.88882338151734</v>
+        <v>964.88882169024339</v>
       </c>
       <c r="H6">
-        <v>74.81186942671296</v>
+        <v>74.811888682028169</v>
       </c>
       <c r="I6">
-        <v>13.401717805426239</v>
+        <v>13.400003353681761</v>
       </c>
       <c r="J6">
-        <v>1468.4398847014936</v>
+        <v>1273.7205982263815</v>
       </c>
       <c r="K6">
-        <v>-3.7380744457714575E-10</v>
+        <v>-3.2827068302375881E-10</v>
       </c>
       <c r="L6">
         <v>-60</v>
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>13.401717805426239</v>
+        <v>13.400003353681761</v>
       </c>
       <c r="P6">
         <v>2.2577542121616823</v>
@@ -1015,19 +1015,19 @@
         <v>2.0580000000000003</v>
       </c>
       <c r="G7">
-        <v>421.76128762635472</v>
+        <v>421.76128744832067</v>
       </c>
       <c r="H7">
-        <v>53.834250142366173</v>
+        <v>53.834249902219547</v>
       </c>
       <c r="I7">
-        <v>2.1683805007596577</v>
+        <v>2.1681142742195001</v>
       </c>
       <c r="J7">
-        <v>970.59278563392297</v>
+        <v>970.59278563297494</v>
       </c>
       <c r="K7">
-        <v>1.0419807399748198E-8</v>
+        <v>1.0419807339439452E-8</v>
       </c>
       <c r="L7">
         <v>-60</v>
@@ -1039,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>2.1683805007596577</v>
+        <v>2.1681142742195001</v>
       </c>
       <c r="P7">
         <v>2.1367296848367752</v>
@@ -1083,19 +1083,19 @@
         <v>2.21</v>
       </c>
       <c r="G8">
-        <v>278.49823038262019</v>
+        <v>278.49822985129339</v>
       </c>
       <c r="H8">
-        <v>26.297105824708328</v>
+        <v>26.297106843548995</v>
       </c>
       <c r="I8">
-        <v>2.335391876121987</v>
+        <v>2.3347051051593266</v>
       </c>
       <c r="J8">
-        <v>970.59278625362197</v>
+        <v>970.59278625091144</v>
       </c>
       <c r="K8">
-        <v>1.041980745569303E-8</v>
+        <v>1.0419807329654527E-8</v>
       </c>
       <c r="L8">
         <v>-60</v>
@@ -1107,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>2.335391876121987</v>
+        <v>2.3347051051593266</v>
       </c>
       <c r="P8">
         <v>3.3675065648772344</v>
@@ -1151,19 +1151,19 @@
         <v>11.015200000000002</v>
       </c>
       <c r="G9">
-        <v>964.88869917520151</v>
+        <v>964.88869653406766</v>
       </c>
       <c r="H9">
-        <v>74.813658551431971</v>
+        <v>74.813682576139243</v>
       </c>
       <c r="I9">
-        <v>11.752059621817782</v>
+        <v>11.749063647516842</v>
       </c>
       <c r="J9">
-        <v>2640.3081292059028</v>
+        <v>1555.5651822845109</v>
       </c>
       <c r="K9">
-        <v>2.7539838294205119E-10</v>
+        <v>2.0197099284881638E-10</v>
       </c>
       <c r="L9">
         <v>-60</v>
@@ -1175,7 +1175,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>11.752059621817782</v>
+        <v>11.749063647516842</v>
       </c>
       <c r="P9">
         <v>3.1770497211103974</v>
@@ -1287,19 +1287,19 @@
         <v>2.8518000000000003</v>
       </c>
       <c r="G11">
-        <v>964.88854771612228</v>
+        <v>964.88854770721957</v>
       </c>
       <c r="H11">
-        <v>74.815033288348843</v>
+        <v>74.815033377504776</v>
       </c>
       <c r="I11">
-        <v>3.0495441317618215</v>
+        <v>3.0495049274861405</v>
       </c>
       <c r="J11">
-        <v>970.59278942152343</v>
+        <v>1057.5532878325171</v>
       </c>
       <c r="K11">
-        <v>1.0419807403732641E-8</v>
+        <v>-1.4166384473778876E-9</v>
       </c>
       <c r="L11">
         <v>-60</v>
@@ -1311,7 +1311,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>3.0495441317618215</v>
+        <v>3.0495049274861405</v>
       </c>
       <c r="P11">
         <v>0.7143478013034501</v>
@@ -1355,19 +1355,19 @@
         <v>0.37240000000000006</v>
       </c>
       <c r="G12">
-        <v>473.28884901734483</v>
+        <v>473.28884901725036</v>
       </c>
       <c r="H12">
-        <v>45.092370491063313</v>
+        <v>45.092370491185598</v>
       </c>
       <c r="I12">
-        <v>0.39249357227766013</v>
+        <v>0.39249235889455036</v>
       </c>
       <c r="J12">
-        <v>970.59278188752467</v>
+        <v>970.59278188751932</v>
       </c>
       <c r="K12">
-        <v>1.0419807397037692E-8</v>
+        <v>1.0419807396522696E-8</v>
       </c>
       <c r="L12">
         <v>-60</v>
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>0.39249357227766013</v>
+        <v>0.39249235889455036</v>
       </c>
       <c r="P12">
         <v>0.34469225101316964</v>
@@ -1423,19 +1423,19 @@
         <v>9.231600000000002</v>
       </c>
       <c r="G13">
-        <v>964.88871191524186</v>
+        <v>964.88871178035379</v>
       </c>
       <c r="H13">
-        <v>74.812950647122634</v>
+        <v>74.812952331288031</v>
       </c>
       <c r="I13">
-        <v>9.9370259733224859</v>
+        <v>9.9368399301019323</v>
       </c>
       <c r="J13">
-        <v>1159.3170658306813</v>
+        <v>1124.7115291208486</v>
       </c>
       <c r="K13">
-        <v>6.0470358634197102E-10</v>
+        <v>-1.4232604389657126E-9</v>
       </c>
       <c r="L13">
         <v>-60</v>
@@ -1447,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>9.9370259733224859</v>
+        <v>9.9368399301019323</v>
       </c>
       <c r="P13">
         <v>0.86496146254423367</v>
@@ -1491,19 +1491,19 @@
         <v>18.737600000000004</v>
       </c>
       <c r="G14">
-        <v>964.88928153288055</v>
+        <v>964.88928064066693</v>
       </c>
       <c r="H14">
-        <v>74.805650097005241</v>
+        <v>74.805661459739568</v>
       </c>
       <c r="I14">
-        <v>20.182549049010248</v>
+        <v>20.181941844009138</v>
       </c>
       <c r="J14">
-        <v>2682.8508105830679</v>
+        <v>2764.9691170165443</v>
       </c>
       <c r="K14">
-        <v>3.3092476398125879E-10</v>
+        <v>9.48539401295092E-11</v>
       </c>
       <c r="L14">
         <v>-60</v>
@@ -1515,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>20.182549049010248</v>
+        <v>20.181941844009138</v>
       </c>
       <c r="P14">
         <v>1.0969792064708848</v>
@@ -1559,19 +1559,19 @@
         <v>7.3892000000000007</v>
       </c>
       <c r="G15">
-        <v>964.88864774092247</v>
+        <v>964.88864767771622</v>
       </c>
       <c r="H15">
-        <v>74.813759046526911</v>
+        <v>74.813759832252344</v>
       </c>
       <c r="I15">
-        <v>7.9526130544060614</v>
+        <v>7.9525041612801468</v>
       </c>
       <c r="J15">
-        <v>1338.9807124916722</v>
+        <v>1338.9802235312629</v>
       </c>
       <c r="K15">
-        <v>-2.2486144722030136E-10</v>
+        <v>-9.1248638888952726E-11</v>
       </c>
       <c r="L15">
         <v>-60</v>
@@ -1583,7 +1583,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>7.9526130544060614</v>
+        <v>7.9525041612801468</v>
       </c>
       <c r="P15">
         <v>0.73964612772368377</v>
@@ -1627,19 +1627,19 @@
         <v>1.5484000000000002</v>
       </c>
       <c r="G16">
-        <v>421.76129159610463</v>
+        <v>421.76129154565768</v>
       </c>
       <c r="H16">
-        <v>53.834247451610452</v>
+        <v>53.834247425615516</v>
       </c>
       <c r="I16">
-        <v>1.6439173193557928</v>
+        <v>1.6438156844787695</v>
       </c>
       <c r="J16">
-        <v>970.59278398685319</v>
+        <v>970.59278398657909</v>
       </c>
       <c r="K16">
-        <v>1.041980744330602E-8</v>
+        <v>1.0419807430241384E-8</v>
       </c>
       <c r="L16">
         <v>-60</v>
@@ -1651,7 +1651,7 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>1.6439173193557928</v>
+        <v>1.6438156844787695</v>
       </c>
       <c r="P16">
         <v>1.5229111097674977</v>
@@ -1695,19 +1695,19 @@
         <v>2.3520000000000003</v>
       </c>
       <c r="G17">
-        <v>616.04467794214827</v>
+        <v>616.0446778605924</v>
       </c>
       <c r="H17">
-        <v>64.774596643737524</v>
+        <v>64.774596627603202</v>
       </c>
       <c r="I17">
-        <v>2.4738509630360879</v>
+        <v>2.4736579087627897</v>
       </c>
       <c r="J17">
-        <v>970.59278680211412</v>
+        <v>970.59278680135913</v>
       </c>
       <c r="K17">
-        <v>1.0419807296938727E-8</v>
+        <v>1.0419807407500243E-8</v>
       </c>
       <c r="L17">
         <v>-60</v>
@@ -1719,7 +1719,7 @@
         <v>0</v>
       </c>
       <c r="O17">
-        <v>2.4738509630360879</v>
+        <v>2.4736579087627897</v>
       </c>
       <c r="P17">
         <v>1.7213459986255004</v>
@@ -1763,19 +1763,19 @@
         <v>11.279800000000002</v>
       </c>
       <c r="G18">
-        <v>964.88880518137353</v>
+        <v>964.88880505448697</v>
       </c>
       <c r="H18">
-        <v>74.811722856105362</v>
+        <v>74.811724470121632</v>
       </c>
       <c r="I18">
-        <v>12.14907527107299</v>
+        <v>12.148931852528131</v>
       </c>
       <c r="J18">
-        <v>2708.7983118464754</v>
+        <v>1362.2980919322511</v>
       </c>
       <c r="K18">
-        <v>1.541267112547455E-10</v>
+        <v>2.2401638874640371E-10</v>
       </c>
       <c r="L18">
         <v>-60</v>
@@ -1787,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>12.14907527107299</v>
+        <v>12.148931852528131</v>
       </c>
       <c r="P18">
         <v>0.68705617240035788</v>
@@ -1831,19 +1831,19 @@
         <v>18.257400000000004</v>
       </c>
       <c r="G19">
-        <v>964.88918997934377</v>
+        <v>964.88918494834752</v>
       </c>
       <c r="H19">
-        <v>74.807348314114719</v>
+        <v>74.807408220819568</v>
       </c>
       <c r="I19">
-        <v>19.625673516085332</v>
+        <v>19.622175803443472</v>
       </c>
       <c r="J19">
-        <v>2661.902697733894</v>
+        <v>2763.1200801819646</v>
       </c>
       <c r="K19">
-        <v>3.8358256458846791E-10</v>
+        <v>9.2573334085842576E-11</v>
       </c>
       <c r="L19">
         <v>-60</v>
@@ -1855,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <v>19.625673516085332</v>
+        <v>19.622175803443472</v>
       </c>
       <c r="P19">
         <v>2.6669440174759429</v>
@@ -1899,19 +1899,19 @@
         <v>11.642400000000002</v>
       </c>
       <c r="G20">
-        <v>964.88876651303963</v>
+        <v>964.88876465564817</v>
       </c>
       <c r="H20">
-        <v>74.812670861443991</v>
+        <v>74.812690766102605</v>
       </c>
       <c r="I20">
-        <v>12.475160347433974</v>
+        <v>12.473148749000446</v>
       </c>
       <c r="J20">
-        <v>2674.8754161982774</v>
+        <v>2713.9457906656512</v>
       </c>
       <c r="K20">
-        <v>2.2002590050442099E-10</v>
+        <v>1.0162290173411643E-10</v>
       </c>
       <c r="L20">
         <v>-60</v>
@@ -1923,7 +1923,7 @@
         <v>0</v>
       </c>
       <c r="O20">
-        <v>12.475160347433974</v>
+        <v>12.473148749000446</v>
       </c>
       <c r="P20">
         <v>2.5324667381562982</v>
@@ -1967,19 +1967,19 @@
         <v>7.1736000000000013</v>
       </c>
       <c r="G21">
-        <v>964.88864326542819</v>
+        <v>964.88864323205053</v>
       </c>
       <c r="H21">
-        <v>74.813794837360874</v>
+        <v>74.813795258566671</v>
       </c>
       <c r="I21">
-        <v>7.7243138631023456</v>
+        <v>7.7242545641359159</v>
       </c>
       <c r="J21">
-        <v>1137.5558097438584</v>
+        <v>1436.1224525572404</v>
       </c>
       <c r="K21">
-        <v>6.5796688754694911E-10</v>
+        <v>-1.1671319686427043E-9</v>
       </c>
       <c r="L21">
         <v>-60</v>
@@ -1991,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="O21">
-        <v>7.7243138631023456</v>
+        <v>7.7242545641359159</v>
       </c>
       <c r="P21">
         <v>0.55396022614012119</v>
@@ -2035,19 +2035,19 @@
         <v>3.0086000000000004</v>
       </c>
       <c r="G22">
-        <v>964.88854966560007</v>
+        <v>964.88854965561848</v>
       </c>
       <c r="H22">
-        <v>74.815009864657128</v>
+        <v>74.815009967317621</v>
       </c>
       <c r="I22">
-        <v>3.2195416042945957</v>
+        <v>3.2194998734757645</v>
       </c>
       <c r="J22">
-        <v>1062.2355830163558</v>
+        <v>1161.4308784227276</v>
       </c>
       <c r="K22">
-        <v>-2.2053187999478748E-10</v>
+        <v>5.484154367584804E-10</v>
       </c>
       <c r="L22">
         <v>-60</v>
@@ -2059,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="O22">
-        <v>3.2195416042945957</v>
+        <v>3.2194998734757645</v>
       </c>
       <c r="P22">
         <v>0.71754839180542296</v>
@@ -2103,19 +2103,19 @@
         <v>4.9294000000000011</v>
       </c>
       <c r="G23">
-        <v>964.88857654747244</v>
+        <v>964.88857648858027</v>
       </c>
       <c r="H23">
-        <v>74.814713295142425</v>
+        <v>74.814713927879978</v>
       </c>
       <c r="I23">
-        <v>5.2817037656136305</v>
+        <v>5.2815531048241402</v>
       </c>
       <c r="J23">
-        <v>1104.849921619199</v>
+        <v>1104.8488931079476</v>
       </c>
       <c r="K23">
-        <v>-8.4179267142585563E-10</v>
+        <v>9.657426235165033E-10</v>
       </c>
       <c r="L23">
         <v>-60</v>
@@ -2127,7 +2127,7 @@
         <v>0</v>
       </c>
       <c r="O23">
-        <v>5.2817037656136305</v>
+        <v>5.2815531048241402</v>
       </c>
       <c r="P23">
         <v>1.0651425852178873</v>
@@ -2171,19 +2171,19 @@
         <v>3.9592000000000005</v>
       </c>
       <c r="G24">
-        <v>655.09800811180151</v>
+        <v>655.0980073890463</v>
       </c>
       <c r="H24">
-        <v>90.271618882562706</v>
+        <v>90.271617499368674</v>
       </c>
       <c r="I24">
-        <v>4.1617206425261237</v>
+        <v>4.1609241773326486</v>
       </c>
       <c r="J24">
-        <v>985.3916138384642</v>
+        <v>1084.345043995366</v>
       </c>
       <c r="K24">
-        <v>2.818643873990286E-10</v>
+        <v>7.0484870460466807E-10</v>
       </c>
       <c r="L24">
         <v>-60</v>
@@ -2195,7 +2195,7 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <v>4.1617206425261237</v>
+        <v>4.1609241773326486</v>
       </c>
       <c r="P24">
         <v>2.6500679504403895</v>
@@ -2239,19 +2239,19 @@
         <v>11.142600000000002</v>
       </c>
       <c r="G25">
-        <v>964.88879673119368</v>
+        <v>964.8887965567028</v>
       </c>
       <c r="H25">
-        <v>74.811849965609525</v>
+        <v>74.811852171993678</v>
       </c>
       <c r="I25">
-        <v>11.998977174955817</v>
+        <v>11.998777589526354</v>
       </c>
       <c r="J25">
-        <v>1854.9271610363492</v>
+        <v>1954.0513283830689</v>
       </c>
       <c r="K25">
-        <v>-1.0768591502512206E-10</v>
+        <v>-8.1452846636326227E-11</v>
       </c>
       <c r="L25">
         <v>-60</v>
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>11.998977174955817</v>
+        <v>11.998777589526354</v>
       </c>
       <c r="P25">
         <v>0.81547251145974264</v>
@@ -2307,19 +2307,19 @@
         <v>5.6056000000000008</v>
       </c>
       <c r="G26">
-        <v>933.99325128669739</v>
+        <v>933.99325073901957</v>
       </c>
       <c r="H26">
-        <v>77.491036743316656</v>
+        <v>77.491038248343827</v>
       </c>
       <c r="I26">
-        <v>5.8927578284774143</v>
+        <v>5.8916905519731104</v>
       </c>
       <c r="J26">
-        <v>1114.2568793473195</v>
+        <v>1015.1743177040878</v>
       </c>
       <c r="K26">
-        <v>2.3590254956933913E-10</v>
+        <v>-5.4153244412746727E-10</v>
       </c>
       <c r="L26">
         <v>-60</v>
@@ -2331,7 +2331,7 @@
         <v>0</v>
       </c>
       <c r="O26">
-        <v>5.8927578284774143</v>
+        <v>5.8916905519731104</v>
       </c>
       <c r="P26">
         <v>2.6504213747458651</v>
@@ -2375,19 +2375,19 @@
         <v>2.9204000000000003</v>
       </c>
       <c r="G27">
-        <v>964.88854073927814</v>
+        <v>964.88854071567107</v>
       </c>
       <c r="H27">
-        <v>74.815124457131731</v>
+        <v>74.81512460443102</v>
       </c>
       <c r="I27">
-        <v>3.0897500224106174</v>
+        <v>3.0896506469680207</v>
       </c>
       <c r="J27">
-        <v>1157.8746189869605</v>
+        <v>970.59278962432313</v>
       </c>
       <c r="K27">
-        <v>6.1014888042877422E-10</v>
+        <v>1.0419807424657743E-8</v>
       </c>
       <c r="L27">
         <v>-60</v>
@@ -2399,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>3.0897500224106174</v>
+        <v>3.0896506469680207</v>
       </c>
       <c r="P27">
         <v>1.1237106940141237</v>
@@ -2443,19 +2443,19 @@
         <v>2.9988000000000006</v>
       </c>
       <c r="G28">
-        <v>964.88854828391754</v>
+        <v>964.88854827156547</v>
       </c>
       <c r="H28">
-        <v>74.815032440735692</v>
+        <v>74.815032559851218</v>
       </c>
       <c r="I28">
-        <v>3.2034547828413027</v>
+        <v>3.2034031541909664</v>
       </c>
       <c r="J28">
-        <v>1061.8027426756994</v>
+        <v>970.59279021413749</v>
       </c>
       <c r="K28">
-        <v>-3.7867167117372203E-10</v>
+        <v>1.0419807374486287E-8</v>
       </c>
       <c r="L28">
         <v>-60</v>
@@ -2467,7 +2467,7 @@
         <v>0</v>
       </c>
       <c r="O28">
-        <v>3.2034547828413027</v>
+        <v>3.2034031541909664</v>
       </c>
       <c r="P28">
         <v>0.79941043356034458</v>
@@ -2511,19 +2511,19 @@
         <v>10.221400000000001</v>
       </c>
       <c r="G29">
-        <v>964.88872804299615</v>
+        <v>964.88872728460217</v>
       </c>
       <c r="H29">
-        <v>74.812957287252473</v>
+        <v>74.81296592386127</v>
       </c>
       <c r="I29">
-        <v>10.9713589889361</v>
+        <v>10.970419906812999</v>
       </c>
       <c r="J29">
-        <v>2671.6142466358824</v>
+        <v>1944.924695456825</v>
       </c>
       <c r="K29">
-        <v>1.9939571669765544E-10</v>
+        <v>-1.4778067407646721E-10</v>
       </c>
       <c r="L29">
         <v>-60</v>
@@ -2535,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="O29">
-        <v>10.9713589889361</v>
+        <v>10.970419906812999</v>
       </c>
       <c r="P29">
         <v>1.8467493551032486</v>
@@ -2579,19 +2579,19 @@
         <v>1.3916000000000002</v>
       </c>
       <c r="G30">
-        <v>186.87270608261613</v>
+        <v>186.87270558583845</v>
       </c>
       <c r="H30">
-        <v>40.180914115173088</v>
+        <v>40.180913491260469</v>
       </c>
       <c r="I30">
-        <v>1.5184932295871971</v>
+        <v>1.5182151582236156</v>
       </c>
       <c r="J30">
-        <v>970.59278366012438</v>
+        <v>970.59278365941088</v>
       </c>
       <c r="K30">
-        <v>1.0419807446721257E-8</v>
+        <v>1.0419807436529756E-8</v>
       </c>
       <c r="L30">
         <v>-60</v>
@@ -2603,7 +2603,7 @@
         <v>0</v>
       </c>
       <c r="O30">
-        <v>1.5184932295871971</v>
+        <v>1.5182151582236156</v>
       </c>
       <c r="P30">
         <v>2.5480114419962745</v>
@@ -2647,19 +2647,19 @@
         <v>4.5374000000000008</v>
       </c>
       <c r="G31">
-        <v>933.99325069382519</v>
+        <v>933.99325046175659</v>
       </c>
       <c r="H31">
-        <v>77.491038054147367</v>
+        <v>77.49103871671052</v>
       </c>
       <c r="I31">
-        <v>4.7713448069355655</v>
+        <v>4.7707857025662772</v>
       </c>
       <c r="J31">
-        <v>1096.1182949203883</v>
+        <v>997.10009259745311</v>
       </c>
       <c r="K31">
-        <v>-1.2506808819957451E-9</v>
+        <v>-3.6702085090052558E-10</v>
       </c>
       <c r="L31">
         <v>-60</v>
@@ -2671,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="O31">
-        <v>4.7713448069355655</v>
+        <v>4.7707857025662772</v>
       </c>
       <c r="P31">
         <v>2.132302591982465</v>
@@ -2715,19 +2715,19 @@
         <v>1.4210000000000003</v>
       </c>
       <c r="G32">
-        <v>278.49822404676121</v>
+        <v>278.49822395790767</v>
       </c>
       <c r="H32">
-        <v>26.297117404078548</v>
+        <v>26.297117588981369</v>
       </c>
       <c r="I32">
-        <v>1.5024828868806321</v>
+        <v>1.5023040163036467</v>
       </c>
       <c r="J32">
-        <v>970.59278362027896</v>
+        <v>970.59278361985639</v>
       </c>
       <c r="K32">
-        <v>1.0419807474070257E-8</v>
+        <v>1.0419807463228235E-8</v>
       </c>
       <c r="L32">
         <v>-60</v>
@@ -2739,7 +2739,7 @@
         <v>0</v>
       </c>
       <c r="O32">
-        <v>1.5024828868806321</v>
+        <v>1.5023040163036467</v>
       </c>
       <c r="P32">
         <v>2.1434788496065242</v>
@@ -2783,19 +2783,19 @@
         <v>3.8906000000000005</v>
       </c>
       <c r="G33">
-        <v>964.88855883211966</v>
+        <v>964.88855880233905</v>
       </c>
       <c r="H33">
-        <v>74.814919157394371</v>
+        <v>74.814919458513899</v>
       </c>
       <c r="I33">
-        <v>4.1615018566052209</v>
+        <v>4.1614056656251428</v>
       </c>
       <c r="J33">
-        <v>985.38737635073653</v>
+        <v>1382.6695706314126</v>
       </c>
       <c r="K33">
-        <v>1.0583121146627351E-9</v>
+        <v>1.2465416373625834E-9</v>
       </c>
       <c r="L33">
         <v>-60</v>
@@ -2807,7 +2807,7 @@
         <v>0</v>
       </c>
       <c r="O33">
-        <v>4.1615018566052209</v>
+        <v>4.1614056656251428</v>
       </c>
       <c r="P33">
         <v>0.95799035983516656</v>
@@ -2851,19 +2851,19 @@
         <v>8.6044000000000018</v>
       </c>
       <c r="G34">
-        <v>964.88864161078618</v>
+        <v>964.88864074037622</v>
       </c>
       <c r="H34">
-        <v>74.814140874736992</v>
+        <v>74.814149158790897</v>
       </c>
       <c r="I34">
-        <v>9.1895925250503279</v>
+        <v>9.1883255227452736</v>
       </c>
       <c r="J34">
-        <v>1053.3825394026182</v>
+        <v>1251.9442881198179</v>
       </c>
       <c r="K34">
-        <v>-1.1940753485748233E-9</v>
+        <v>4.70070796307977E-10</v>
       </c>
       <c r="L34">
         <v>-60</v>
@@ -2875,7 +2875,7 @@
         <v>0</v>
       </c>
       <c r="O34">
-        <v>9.1895925250503279</v>
+        <v>9.1883255227452736</v>
       </c>
       <c r="P34">
         <v>2.3377851878514901</v>
@@ -2919,19 +2919,19 @@
         <v>3.5378000000000007</v>
       </c>
       <c r="G35">
-        <v>757.74013130810215</v>
+        <v>757.74013105488939</v>
       </c>
       <c r="H35">
-        <v>86.869471326886611</v>
+        <v>86.869471052109333</v>
       </c>
       <c r="I35">
-        <v>3.7159699893297105</v>
+        <v>3.715525875401787</v>
       </c>
       <c r="J35">
-        <v>975.6655932115691</v>
+        <v>1074.5932768852201</v>
       </c>
       <c r="K35">
-        <v>-1.4793736184780094E-9</v>
+        <v>1.3871111094382881E-10</v>
       </c>
       <c r="L35">
         <v>-60</v>
@@ -2943,7 +2943,7 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <v>3.7159699893297105</v>
+        <v>3.715525875401787</v>
       </c>
       <c r="P35">
         <v>2.1183837263904857</v>
@@ -2987,19 +2987,19 @@
         <v>16.473800000000001</v>
       </c>
       <c r="G36">
-        <v>964.88907506157523</v>
+        <v>964.88907219871851</v>
       </c>
       <c r="H36">
-        <v>74.808645733412064</v>
+        <v>74.808680221694246</v>
       </c>
       <c r="I36">
-        <v>17.713936020296618</v>
+        <v>17.711728456662104</v>
       </c>
       <c r="J36">
-        <v>1788.9655560614408</v>
+        <v>1607.7397613682006</v>
       </c>
       <c r="K36">
-        <v>4.248448781725237E-10</v>
+        <v>-1.0589158246699423E-9</v>
       </c>
       <c r="L36">
         <v>-60</v>
@@ -3011,7 +3011,7 @@
         <v>0</v>
       </c>
       <c r="O36">
-        <v>17.713936020296618</v>
+        <v>17.711728456662104</v>
       </c>
       <c r="P36">
         <v>2.2304969312426666</v>
@@ -3055,19 +3055,19 @@
         <v>2.5480000000000005</v>
       </c>
       <c r="G37">
-        <v>616.04468098287487</v>
+        <v>616.04468087569649</v>
       </c>
       <c r="H37">
-        <v>64.774595331191193</v>
+        <v>64.774595349560698</v>
       </c>
       <c r="I37">
-        <v>2.6860142775201732</v>
+        <v>2.685779143800302</v>
       </c>
       <c r="J37">
-        <v>1046.6094381136468</v>
+        <v>1046.6031240474372</v>
       </c>
       <c r="K37">
-        <v>-1.4407995813703616E-9</v>
+        <v>1.2651717421156755E-9</v>
       </c>
       <c r="L37">
         <v>-60</v>
@@ -3079,7 +3079,7 @@
         <v>0</v>
       </c>
       <c r="O37">
-        <v>2.6860142775201732</v>
+        <v>2.685779143800302</v>
       </c>
       <c r="P37">
         <v>1.8253803547622955</v>
@@ -3123,19 +3123,19 @@
         <v>14.866600000000002</v>
       </c>
       <c r="G38">
-        <v>964.88897238369441</v>
+        <v>964.88897038019832</v>
       </c>
       <c r="H38">
-        <v>74.809904455026327</v>
+        <v>74.809928497331711</v>
       </c>
       <c r="I38">
-        <v>15.983534723532214</v>
+        <v>15.981823243407925</v>
       </c>
       <c r="J38">
-        <v>1698.7641484280259</v>
+        <v>1680.9620413392272</v>
       </c>
       <c r="K38">
-        <v>9.638344709179573E-10</v>
+        <v>-4.0455244104217884E-11</v>
       </c>
       <c r="L38">
         <v>-60</v>
@@ -3147,7 +3147,7 @@
         <v>0</v>
       </c>
       <c r="O38">
-        <v>15.983534723532214</v>
+        <v>15.981823243407925</v>
       </c>
       <c r="P38">
         <v>2.0673544330144757</v>
@@ -3191,19 +3191,19 @@
         <v>6.0760000000000005</v>
       </c>
       <c r="G39">
-        <v>964.88857479012165</v>
+        <v>964.88857446814643</v>
       </c>
       <c r="H39">
-        <v>74.814842029811473</v>
+        <v>74.814844591335628</v>
       </c>
       <c r="I39">
-        <v>6.4607326144868784</v>
+        <v>6.460074738597382</v>
       </c>
       <c r="J39">
-        <v>1122.1671551514592</v>
+        <v>1023.0688600437626</v>
       </c>
       <c r="K39">
-        <v>5.9724377668417267E-10</v>
+        <v>7.427039826830365E-10</v>
       </c>
       <c r="L39">
         <v>-60</v>
@@ -3215,7 +3215,7 @@
         <v>0</v>
       </c>
       <c r="O39">
-        <v>6.4607326144868784</v>
+        <v>6.460074738597382</v>
       </c>
       <c r="P39">
         <v>2.004574802018523</v>

</xml_diff>